<commit_message>
UPGRADE name of valuer/ref
</commit_message>
<xml_diff>
--- a/Documents/GameDesign/System_Design.xlsx
+++ b/Documents/GameDesign/System_Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin DIJOUX\Documents\Unity\Workshop_TowerDefense\STD_Workshop\Documents\GameDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74950E5-677B-4267-8A0E-757ACA540770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278BB47F-6B6F-45A9-B616-212B21662E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EE4EEEAB-A39E-4793-9971-E358DB8AAF6E}"/>
   </bookViews>
@@ -350,10 +350,10 @@
     <t>arrondi #,##</t>
   </si>
   <si>
-    <t>Valeur Modifiable</t>
-  </si>
-  <si>
     <t>List</t>
+  </si>
+  <si>
+    <t>Valeur Ref</t>
   </si>
 </sst>
 </file>
@@ -845,47 +845,38 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -901,9 +892,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -936,9 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -963,37 +948,52 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1679,31 +1679,31 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25:F25"/>
+      <selection activeCell="Q2" sqref="Q2:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="65"/>
-    <col min="2" max="2" width="22.42578125" style="66" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="66" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="66" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="66"/>
-    <col min="6" max="6" width="5.7109375" style="66" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="66"/>
-    <col min="8" max="8" width="5.7109375" style="66" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="66"/>
-    <col min="10" max="10" width="5.7109375" style="66" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="66"/>
-    <col min="12" max="12" width="5.7109375" style="66" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="66"/>
-    <col min="14" max="14" width="5.7109375" style="66" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="66" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.28515625" style="66" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" style="70" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="66" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="70" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="66"/>
+    <col min="1" max="1" width="11.42578125" style="61"/>
+    <col min="2" max="2" width="22.42578125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="62" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="62" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="62"/>
+    <col min="6" max="6" width="5.7109375" style="62" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="62"/>
+    <col min="8" max="8" width="5.7109375" style="62" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="62"/>
+    <col min="10" max="10" width="5.7109375" style="62" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="62"/>
+    <col min="12" max="12" width="5.7109375" style="62" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="62"/>
+    <col min="14" max="14" width="5.7109375" style="62" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="62" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" style="62" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" style="66" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="62" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" style="66" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="62"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1711,388 +1711,388 @@
         <v>15</v>
       </c>
       <c r="B1" s="41"/>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="60" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="G1" s="60" t="s">
+      <c r="F1" s="58"/>
+      <c r="G1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="60" t="s">
+      <c r="H1" s="58"/>
+      <c r="I1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="60" t="s">
+      <c r="J1" s="58"/>
+      <c r="K1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="61"/>
-      <c r="M1" s="60" t="s">
+      <c r="L1" s="58"/>
+      <c r="M1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="69"/>
-      <c r="O1" s="91" t="s">
+      <c r="N1" s="65"/>
+      <c r="O1" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="95" t="s">
-        <v>90</v>
-      </c>
-      <c r="R1" s="95"/>
+      <c r="Q1" s="85" t="s">
+        <v>91</v>
+      </c>
+      <c r="R1" s="85"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="95" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="58">
+      <c r="C2" s="55">
         <f>$D$16</f>
         <v>1</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="58" cm="1">
+      <c r="E2" s="55" cm="1">
         <f t="array" ref="E2">_xlfn.IFS(D2="+",ROUNDDOWN(C2*$O$2,2),D2="=",C2)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="58" cm="1">
+      <c r="G2" s="55" cm="1">
         <f t="array" ref="G2">_xlfn.IFS(F2="+",ROUNDDOWN(E2*$O$2,2),F2="=",E2)</f>
         <v>1.21</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="58" cm="1">
+      <c r="I2" s="55" cm="1">
         <f t="array" ref="I2">_xlfn.IFS(H2="+",ROUNDDOWN(G2*$O$2,2),H2="=",G2)</f>
         <v>1.33</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="J2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="58" cm="1">
+      <c r="K2" s="55" cm="1">
         <f t="array" ref="K2">_xlfn.IFS(J2="+",ROUNDDOWN(I2*$O$2,2),J2="=",I2)</f>
         <v>1.46</v>
       </c>
-      <c r="L2" s="58" t="s">
+      <c r="L2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="58" cm="1">
+      <c r="M2" s="55" cm="1">
         <f t="array" ref="M2">_xlfn.IFS(L2="+",ROUNDDOWN(K2*$O$2,2),L2="=",K2)</f>
         <v>1.6</v>
       </c>
-      <c r="O2" s="58">
+      <c r="O2" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q2" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="R2" s="96"/>
-      <c r="S2" s="66"/>
+      <c r="Q2" s="86" t="s">
+        <v>90</v>
+      </c>
+      <c r="R2" s="86"/>
+      <c r="S2" s="62"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
+      <c r="A3" s="95"/>
       <c r="B3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="59">
+      <c r="C3" s="56">
         <f>$F$16</f>
         <v>0.5</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="59" cm="1">
+      <c r="E3" s="56" cm="1">
         <f t="array" ref="E3">_xlfn.IFS(D3="+",ROUNDDOWN(C3*$O$3,2),D3="=",C3)</f>
         <v>0.45</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="59" cm="1">
+      <c r="G3" s="56" cm="1">
         <f t="array" ref="G3">_xlfn.IFS(F3="+",ROUNDDOWN(E3*$O$3,2),F3="=",E3)</f>
         <v>0.4</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="59" cm="1">
+      <c r="I3" s="56" cm="1">
         <f t="array" ref="I3">_xlfn.IFS(H3="+",ROUNDDOWN(G3*$O$3,2),H3="=",G3)</f>
         <v>0.36</v>
       </c>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="59" cm="1">
+      <c r="K3" s="56" cm="1">
         <f t="array" ref="K3">_xlfn.IFS(J3="+",ROUNDDOWN(I3*$O$3,2),J3="=",I3)</f>
         <v>0.32</v>
       </c>
-      <c r="L3" s="59" t="s">
+      <c r="L3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="59" cm="1">
+      <c r="M3" s="56" cm="1">
         <f t="array" ref="M3">_xlfn.IFS(L3="+",ROUNDDOWN(K3*$O$3,2),L3="=",K3)</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="O3" s="59">
+      <c r="O3" s="56">
         <v>0.9</v>
       </c>
-      <c r="Q3" s="96"/>
-      <c r="R3" s="96"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
-      <c r="B4" s="88" t="s">
+      <c r="A4" s="95"/>
+      <c r="B4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="58">
+      <c r="C4" s="55">
         <f>$H$16</f>
         <v>3</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="58" cm="1">
+      <c r="E4" s="55" cm="1">
         <f t="array" ref="E4">_xlfn.IFS(D4="+",ROUNDDOWN(C4*$O$4,2),D4="=",C4)</f>
         <v>3.75</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="58" cm="1">
+      <c r="G4" s="55" cm="1">
         <f t="array" ref="G4">_xlfn.IFS(F4="+",ROUNDDOWN(E4*$O$4,2),F4="=",E4)</f>
         <v>4.68</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="58" cm="1">
+      <c r="I4" s="55" cm="1">
         <f t="array" ref="I4">_xlfn.IFS(H4="+",ROUNDDOWN(G4*$O$4,2),H4="=",G4)</f>
         <v>5.85</v>
       </c>
-      <c r="J4" s="58" t="s">
+      <c r="J4" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="58" cm="1">
+      <c r="K4" s="55" cm="1">
         <f t="array" ref="K4">_xlfn.IFS(J4="+",ROUNDDOWN(I4*$O$4,2),J4="=",I4)</f>
         <v>7.31</v>
       </c>
-      <c r="L4" s="58" t="s">
+      <c r="L4" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="58" cm="1">
+      <c r="M4" s="55" cm="1">
         <f t="array" ref="M4">_xlfn.IFS(L4="+",ROUNDDOWN(K4*$O$4,2),L4="=",K4)</f>
         <v>9.1300000000000008</v>
       </c>
-      <c r="O4" s="58">
+      <c r="O4" s="55">
         <v>1.25</v>
       </c>
-      <c r="S4" s="66"/>
+      <c r="S4" s="62"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+      <c r="A5" s="95"/>
       <c r="B5" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="56">
         <f>$J$16</f>
         <v>15</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="59" cm="1">
+      <c r="E5" s="56" cm="1">
         <f t="array" ref="E5">_xlfn.IFS(D5="+",ROUNDUP(C5*$O$5,0),D5="=",C5)</f>
         <v>15</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="59" cm="1">
+      <c r="G5" s="56" cm="1">
         <f t="array" ref="G5">_xlfn.IFS(F5="+",ROUNDUP(E5*$O$5,0),F5="=",E5)</f>
         <v>15</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="59" cm="1">
+      <c r="I5" s="56" cm="1">
         <f t="array" ref="I5">_xlfn.IFS(H5="+",ROUNDUP(G5*$O$5,0),H5="=",G5)</f>
         <v>15</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="59" cm="1">
+      <c r="K5" s="56" cm="1">
         <f t="array" ref="K5">_xlfn.IFS(J5="+",ROUNDUP(I5*$O$5,0),J5="=",I5)</f>
         <v>15</v>
       </c>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="59" cm="1">
+      <c r="M5" s="56" cm="1">
         <f t="array" ref="M5">_xlfn.IFS(L5="+",ROUNDUP(K5*$O$5,0),L5="=",K5)</f>
         <v>15</v>
       </c>
-      <c r="O5" s="59">
+      <c r="O5" s="56">
         <v>1.5</v>
       </c>
-      <c r="S5" s="66"/>
+      <c r="S5" s="62"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="88" t="s">
+      <c r="A6" s="95"/>
+      <c r="B6" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64">
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60">
         <f>ROUNDDOWN((E2-C2)/C2,2)</f>
         <v>0.1</v>
       </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64">
+      <c r="F6" s="60"/>
+      <c r="G6" s="60">
         <f>ROUNDDOWN((G2-E2)/E2,2)</f>
         <v>0.09</v>
       </c>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64">
+      <c r="H6" s="60"/>
+      <c r="I6" s="60">
         <f>ROUNDDOWN((I2-G2)/G2,2)</f>
         <v>0.09</v>
       </c>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64">
+      <c r="J6" s="60"/>
+      <c r="K6" s="60">
         <f>ROUNDDOWN((K2-I2)/I2,2)</f>
         <v>0.09</v>
       </c>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64">
+      <c r="L6" s="60"/>
+      <c r="M6" s="60">
         <f>ROUNDDOWN((M2-K2)/K2,2)</f>
         <v>0.09</v>
       </c>
-      <c r="N6" s="67"/>
-      <c r="O6" s="70"/>
-      <c r="Q6" s="67"/>
-      <c r="S6" s="66"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="66"/>
+      <c r="Q6" s="63"/>
+      <c r="S6" s="62"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63">
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59">
         <f t="shared" ref="E7:E8" si="0">ROUNDDOWN((E3-C3)/C3,2)</f>
         <v>-0.1</v>
       </c>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63">
+      <c r="F7" s="59"/>
+      <c r="G7" s="59">
         <f t="shared" ref="G7:G8" si="1">ROUNDDOWN((G3-E3)/E3,2)</f>
         <v>-0.11</v>
       </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63">
+      <c r="H7" s="59"/>
+      <c r="I7" s="59">
         <f t="shared" ref="I7:I8" si="2">ROUNDDOWN((I3-G3)/G3,2)</f>
         <v>-0.1</v>
       </c>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63">
+      <c r="J7" s="59"/>
+      <c r="K7" s="59">
         <f>ROUNDDOWN((K3-I3)/I3,2)</f>
         <v>-0.11</v>
       </c>
-      <c r="L7" s="63"/>
-      <c r="M7" s="63">
+      <c r="L7" s="59"/>
+      <c r="M7" s="59">
         <f>ROUNDDOWN((M3-K3)/K3,2)</f>
         <v>-0.12</v>
       </c>
-      <c r="N7" s="67"/>
-      <c r="O7" s="91" t="s">
+      <c r="N7" s="63"/>
+      <c r="O7" s="83" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="88" t="s">
+      <c r="A8" s="95"/>
+      <c r="B8" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64">
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64">
+      <c r="F8" s="60"/>
+      <c r="G8" s="60">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64">
+      <c r="H8" s="60"/>
+      <c r="I8" s="60">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64">
+      <c r="J8" s="60"/>
+      <c r="K8" s="60">
         <f>ROUNDDOWN((K4-I4)/I4,2)</f>
         <v>0.24</v>
       </c>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64">
+      <c r="L8" s="60"/>
+      <c r="M8" s="60">
         <f>ROUNDDOWN((M4-K4)/K4,2)</f>
         <v>0.24</v>
       </c>
-      <c r="O8" s="58">
+      <c r="O8" s="55">
         <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
-      <c r="Q9" s="66"/>
-      <c r="S9" s="66"/>
+      <c r="A9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="S9" s="62"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
+      <c r="A10" s="68"/>
       <c r="B10" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="58">
+      <c r="C10" s="55">
         <f>ROUNDDOWN(C2/C3,2)</f>
         <v>2</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58">
+      <c r="D10" s="55"/>
+      <c r="E10" s="55">
         <f>ROUNDDOWN(E2/E3,2)</f>
         <v>2.44</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58">
+      <c r="F10" s="55"/>
+      <c r="G10" s="55">
         <f>ROUNDDOWN(G2/G3,2)</f>
         <v>3.02</v>
       </c>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58">
+      <c r="H10" s="55"/>
+      <c r="I10" s="55">
         <f>ROUNDDOWN(I2/I3,2)</f>
         <v>3.69</v>
       </c>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58">
+      <c r="J10" s="55"/>
+      <c r="K10" s="55">
         <f>ROUNDDOWN(K2/K3,2)</f>
         <v>4.5599999999999996</v>
       </c>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58">
+      <c r="L10" s="55"/>
+      <c r="M10" s="55">
         <f>ROUNDDOWN(M2/M3,2)</f>
         <v>5.71</v>
       </c>
-      <c r="O10" s="91" t="s">
+      <c r="O10" s="83" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2100,351 +2100,362 @@
       <c r="B11" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="67">
+      <c r="C11" s="63">
         <f>1/C3</f>
         <v>2</v>
       </c>
-      <c r="D11" s="69"/>
-      <c r="E11" s="67">
+      <c r="D11" s="65"/>
+      <c r="E11" s="63">
         <f>1/E3</f>
         <v>2.2222222222222223</v>
       </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="67">
+      <c r="F11" s="65"/>
+      <c r="G11" s="63">
         <f>1/G3</f>
         <v>2.5</v>
       </c>
-      <c r="H11" s="69"/>
-      <c r="I11" s="67">
+      <c r="H11" s="65"/>
+      <c r="I11" s="63">
         <f>1/I3</f>
         <v>2.7777777777777777</v>
       </c>
-      <c r="J11" s="69"/>
-      <c r="K11" s="67">
+      <c r="J11" s="65"/>
+      <c r="K11" s="63">
         <f>1/K3</f>
         <v>3.125</v>
       </c>
-      <c r="L11" s="69"/>
-      <c r="M11" s="67">
+      <c r="L11" s="65"/>
+      <c r="M11" s="63">
         <f>1/M3</f>
         <v>3.5714285714285712</v>
       </c>
-      <c r="O11" s="58">
+      <c r="O11" s="55">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
-      <c r="S12" s="66"/>
+      <c r="A12" s="62"/>
+      <c r="S12" s="62"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
-      <c r="B13" s="73" t="s">
+      <c r="A13" s="62"/>
+      <c r="B13" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="42"/>
-      <c r="S13" s="66"/>
+      <c r="E13" s="94"/>
+      <c r="S13" s="62"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="66"/>
-      <c r="B14" s="57" t="s">
+      <c r="A14" s="62"/>
+      <c r="B14" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="58" t="str">
+      <c r="C14" s="55" t="str">
         <f>VLOOKUP($B$14,ENEMIES,3)</f>
         <v>Insect</v>
       </c>
-      <c r="D14" s="74">
+      <c r="D14" s="91">
         <f>VLOOKUP($B$14,ENEMIES,5)</f>
         <v>5</v>
       </c>
-      <c r="E14" s="74"/>
-      <c r="O14" s="70"/>
+      <c r="E14" s="91"/>
+      <c r="O14" s="66"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="66"/>
-      <c r="B15" s="56" t="s">
+      <c r="A15" s="62"/>
+      <c r="B15" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42" t="s">
+      <c r="E15" s="94"/>
+      <c r="F15" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42" t="s">
+      <c r="G15" s="94"/>
+      <c r="H15" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42" t="s">
+      <c r="I15" s="94"/>
+      <c r="J15" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="42"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="70"/>
-      <c r="Q15" s="94"/>
-      <c r="R15" s="94"/>
-      <c r="S15" s="94"/>
-      <c r="T15" s="94"/>
-      <c r="U15" s="94"/>
-      <c r="V15" s="94"/>
+      <c r="K15" s="94"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="66"/>
+      <c r="Q15" s="84"/>
+      <c r="R15" s="84"/>
+      <c r="S15" s="84"/>
+      <c r="T15" s="84"/>
+      <c r="U15" s="84"/>
+      <c r="V15" s="84"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
-      <c r="B16" s="57" t="s">
+      <c r="A16" s="62"/>
+      <c r="B16" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="58" t="str">
+      <c r="C16" s="55" t="str">
         <f>VLOOKUP($B$16,TOWER,3)</f>
         <v>Traps</v>
       </c>
-      <c r="D16" s="74">
+      <c r="D16" s="91">
         <f>VLOOKUP($B$16,TOWER,4)</f>
         <v>1</v>
       </c>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74">
+      <c r="E16" s="91"/>
+      <c r="F16" s="91">
         <f>VLOOKUP($B$16,TOWER,5)</f>
         <v>0.5</v>
       </c>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74">
+      <c r="G16" s="91"/>
+      <c r="H16" s="91">
         <f>VLOOKUP($B$16,TOWER,6)</f>
         <v>3</v>
       </c>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74">
+      <c r="I16" s="91"/>
+      <c r="J16" s="91">
         <f>VLOOKUP($B$16,TOWER,7)</f>
         <v>15</v>
       </c>
-      <c r="K16" s="74"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="70"/>
-      <c r="Q16" s="67"/>
-      <c r="R16" s="69"/>
-      <c r="S16" s="67"/>
-      <c r="T16" s="67"/>
-      <c r="U16" s="67"/>
-      <c r="V16" s="67"/>
+      <c r="K16" s="91"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="66"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="65"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="63"/>
+      <c r="U16" s="63"/>
+      <c r="V16" s="63"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
-      <c r="N17" s="67"/>
-      <c r="O17" s="70"/>
-      <c r="Q17" s="67"/>
-      <c r="R17" s="69"/>
-      <c r="S17" s="67"/>
-      <c r="T17" s="67"/>
-      <c r="U17" s="67"/>
-      <c r="V17" s="67"/>
+      <c r="A17" s="62"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="66"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="65"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="63"/>
+      <c r="U17" s="63"/>
+      <c r="V17" s="63"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
-      <c r="N18" s="67"/>
-      <c r="O18" s="70"/>
-      <c r="P18" s="67"/>
-      <c r="Q18" s="67"/>
-      <c r="R18" s="67"/>
-      <c r="S18" s="67"/>
-      <c r="T18" s="67"/>
-      <c r="U18" s="67"/>
-      <c r="V18" s="67"/>
+      <c r="A18" s="62"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
+      <c r="R18" s="63"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="63"/>
+      <c r="U18" s="63"/>
+      <c r="V18" s="63"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="86"/>
-      <c r="E19" s="86" t="s">
+      <c r="C19" s="89"/>
+      <c r="E19" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="86"/>
-      <c r="K19" s="60" t="s">
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="89"/>
+      <c r="K19" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="Q19" s="66"/>
-      <c r="S19" s="66"/>
+      <c r="Q19" s="62"/>
+      <c r="S19" s="62"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="74">
+      <c r="B20" s="91">
         <f>O11*K21</f>
         <v>24.4</v>
       </c>
-      <c r="C20" s="74"/>
-      <c r="E20" s="74" t="str">
+      <c r="C20" s="91"/>
+      <c r="E20" s="91" t="str">
         <f>C16</f>
         <v>Traps</v>
       </c>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74" t="str">
+      <c r="F20" s="91"/>
+      <c r="G20" s="91" t="str">
         <f>C14</f>
         <v>Insect</v>
       </c>
-      <c r="H20" s="74"/>
-      <c r="I20" s="58" t="s">
+      <c r="H20" s="91"/>
+      <c r="I20" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="89" t="s">
+      <c r="K20" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="N20" s="71"/>
-      <c r="O20" s="68"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="64"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="86" t="s">
+      <c r="B21" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="86"/>
-      <c r="E21" s="90" t="str">
+      <c r="C21" s="89"/>
+      <c r="E21" s="92" t="str">
         <f>HLOOKUP(C16,TOWER_TYP,VLOOKUP(C14,ENEMY_TYP,5,FALSE)+1,FALSE)</f>
         <v>+</v>
       </c>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="87" cm="1">
+      <c r="F21" s="92"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="93" cm="1">
         <f t="array" ref="I21">_xlfn.IFS(E21="-", 1-O8, E21="=",1,E21="+",1+O8)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="K21" s="87" cm="1">
+      <c r="K21" s="93" cm="1">
         <f t="array" ref="K21">_xlfn.IFS(K20="Upgrade 1",E10,K20="Upgrade 2",G10,K20="Upgrade 3",I10,K20="Upgrade 4",K10,K20="Upgrade 5",M10,K20="Upgrade 6",#REF!)</f>
         <v>2.44</v>
       </c>
-      <c r="O21" s="68"/>
-      <c r="Q21" s="66"/>
-      <c r="S21" s="66"/>
+      <c r="O21" s="64"/>
+      <c r="Q21" s="62"/>
+      <c r="S21" s="62"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="74">
+      <c r="B22" s="91">
         <f>O11*K21</f>
         <v>24.4</v>
       </c>
-      <c r="C22" s="74"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
-      <c r="H22" s="90"/>
-      <c r="I22" s="87"/>
-      <c r="K22" s="87"/>
-      <c r="O22" s="68"/>
-      <c r="Q22" s="66"/>
-      <c r="S22" s="66"/>
+      <c r="C22" s="91"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="93"/>
+      <c r="K22" s="93"/>
+      <c r="O22" s="64"/>
+      <c r="Q22" s="62"/>
+      <c r="S22" s="62"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="N23" s="67"/>
-      <c r="O23" s="68"/>
-      <c r="Q23" s="66"/>
-      <c r="S23" s="66"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="64"/>
+      <c r="Q23" s="62"/>
+      <c r="S23" s="62"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="92"/>
-      <c r="E24" s="92" t="s">
+      <c r="D24" s="90"/>
+      <c r="E24" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="92"/>
-      <c r="N24" s="67"/>
-      <c r="O24" s="68"/>
-      <c r="Q24" s="68"/>
-      <c r="S24" s="66"/>
+      <c r="F24" s="90"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="S24" s="62"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="60" t="str">
+      <c r="B25" s="57" t="str">
         <f>K20</f>
         <v>Upgrade 1</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="88">
         <f>ROUNDDOWN($D$14/(K21*$I$21),2)</f>
         <v>1.86</v>
       </c>
-      <c r="D25" s="43"/>
-      <c r="E25" s="93">
+      <c r="D25" s="88"/>
+      <c r="E25" s="87">
         <f>ROUNDUP($D$14/(K21*$I$21),0)</f>
         <v>2</v>
       </c>
-      <c r="F25" s="93"/>
-      <c r="N25" s="67"/>
-      <c r="O25" s="68"/>
-      <c r="Q25" s="68"/>
-      <c r="S25" s="66"/>
+      <c r="F25" s="87"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="64"/>
+      <c r="Q25" s="64"/>
+      <c r="S25" s="62"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="N26" s="69"/>
-      <c r="O26" s="68"/>
+      <c r="N26" s="65"/>
+      <c r="O26" s="64"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="N27" s="71"/>
-      <c r="O27" s="68"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="64"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="O28" s="68"/>
+      <c r="O28" s="64"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="O29" s="68"/>
+      <c r="O29" s="64"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="O30" s="68"/>
+      <c r="O30" s="64"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="O31" s="68"/>
-      <c r="S31" s="66"/>
+      <c r="O31" s="64"/>
+      <c r="S31" s="62"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="O32" s="68"/>
-      <c r="S32" s="66"/>
+      <c r="O32" s="64"/>
+      <c r="S32" s="62"/>
     </row>
     <row r="33" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="O33" s="68"/>
-      <c r="S33" s="66"/>
+      <c r="O33" s="64"/>
+      <c r="S33" s="62"/>
     </row>
     <row r="34" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q34" s="68"/>
+      <c r="Q34" s="64"/>
     </row>
     <row r="35" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q35" s="68"/>
+      <c r="Q35" s="64"/>
     </row>
     <row r="36" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q36" s="68"/>
+      <c r="Q36" s="64"/>
     </row>
     <row r="37" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q37" s="68"/>
+      <c r="Q37" s="64"/>
     </row>
     <row r="38" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q38" s="68"/>
+      <c r="Q38" s="64"/>
     </row>
     <row r="39" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q39" s="68"/>
+      <c r="Q39" s="64"/>
     </row>
     <row r="40" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q40" s="68"/>
+      <c r="Q40" s="64"/>
     </row>
     <row r="41" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q41" s="68"/>
+      <c r="Q41" s="64"/>
     </row>
     <row r="42" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q42" s="68"/>
+      <c r="Q42" s="64"/>
     </row>
     <row r="43" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q43" s="68"/>
+      <c r="Q43" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="Q2:R3"/>
     <mergeCell ref="E25:F25"/>
@@ -2461,17 +2472,6 @@
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F15:G15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="T17:T18 V17:V18">
@@ -2486,7 +2486,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25 Q18">
+  <conditionalFormatting sqref="Q18 C25">
     <cfRule type="colorScale" priority="145">
       <colorScale>
         <cfvo type="min"/>
@@ -2506,7 +2506,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25 Q18 S17:S18 U17:U18">
+  <conditionalFormatting sqref="Q18 C25 S17:S18 U17:U18">
     <cfRule type="colorScale" priority="151">
       <colorScale>
         <cfvo type="min"/>
@@ -2516,7 +2516,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25 R18">
+  <conditionalFormatting sqref="R18 E25">
     <cfRule type="colorScale" priority="157">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -2950,57 +2950,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76">
+      <c r="A1" s="71">
         <v>1</v>
       </c>
-      <c r="B1" s="76">
+      <c r="B1" s="71">
         <v>2</v>
       </c>
-      <c r="C1" s="76">
+      <c r="C1" s="71">
         <v>3</v>
       </c>
-      <c r="D1" s="76">
+      <c r="D1" s="71">
         <v>4</v>
       </c>
-      <c r="E1" s="76">
+      <c r="E1" s="71">
         <v>5</v>
       </c>
-      <c r="F1" s="76">
+      <c r="F1" s="71">
         <v>6</v>
       </c>
-      <c r="G1" s="76">
+      <c r="G1" s="71">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="80" t="s">
+      <c r="G2" s="75" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="str">
+      <c r="A3" s="76" t="str">
         <f>_xlfn.CONCAT(B3,"_",LEFT(C3,4),)</f>
         <v>1_Food</v>
       </c>
-      <c r="B3" s="82">
+      <c r="B3" s="77">
         <v>1</v>
       </c>
       <c r="C3" s="30" t="s">
@@ -3020,11 +3020,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="str">
+      <c r="A4" s="78" t="str">
         <f>_xlfn.CONCAT(B4,"_",LEFT(C4,4),)</f>
         <v>2_Trap</v>
       </c>
-      <c r="B4" s="75">
+      <c r="B4" s="70">
         <v>2</v>
       </c>
       <c r="C4" s="25" t="s">
@@ -3044,11 +3044,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="84" t="str">
+      <c r="A5" s="79" t="str">
         <f>_xlfn.CONCAT(B5,"_",LEFT(C5,4),)</f>
         <v>3_Ener</v>
       </c>
-      <c r="B5" s="85">
+      <c r="B5" s="80">
         <v>3</v>
       </c>
       <c r="C5" s="31" t="s">
@@ -3156,7 +3156,7 @@
       <c r="B1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="44" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="35" t="s">
@@ -3171,7 +3171,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="45" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="6"/>
@@ -3203,7 +3203,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="46" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="6"/>
@@ -3224,11 +3224,11 @@
       <c r="H5" s="24"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="44" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="44"/>
+      <c r="D6" s="42"/>
       <c r="E6" s="6"/>
       <c r="F6" s="5" t="s">
         <v>13</v>
@@ -3242,7 +3242,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="45"/>
+      <c r="D7" s="43"/>
       <c r="E7" s="6"/>
       <c r="F7" s="8" t="s">
         <v>14</v>
@@ -3329,18 +3329,18 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="16"/>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="47" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="50" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="32" t="s">
@@ -3355,15 +3355,15 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="52" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="49" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="36" t="s">
@@ -3378,14 +3378,14 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" s="55" t="str">
+      <c r="G4" s="96" t="str">
         <f>HLOOKUP(G3,C2:E5,VLOOKUP(H3,B3:F5,5,FALSE)+1,FALSE)</f>
         <v>+</v>
       </c>
-      <c r="H4" s="55"/>
+      <c r="H4" s="96"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="50" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="37" t="s">
@@ -3400,23 +3400,23 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="16"/>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="47" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="50" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="32" t="s">
@@ -3431,15 +3431,15 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="G8" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="52" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="36" t="s">
@@ -3454,14 +3454,14 @@
       <c r="F9">
         <v>2</v>
       </c>
-      <c r="G9" s="55" t="str">
+      <c r="G9" s="96" t="str">
         <f>HLOOKUP(G8,C7:E10,VLOOKUP(H8,B8:F10,5,FALSE)+1,FALSE)</f>
         <v>=</v>
       </c>
-      <c r="H9" s="55"/>
+      <c r="H9" s="96"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="50" t="s">
         <v>84</v>
       </c>
       <c r="C10" s="37" t="s">
@@ -3476,8 +3476,8 @@
       <c r="F10">
         <v>3</v>
       </c>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3663,12 +3663,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100841444F490B10C45A279B0383115D26D" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="91c543cf6706f2108a45fe2b21185738">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c3a97ae1-1078-4f52-97c7-e1e75f184270" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6cf98f67490a83722a01f9dfd5fe46d6" ns3:_="">
     <xsd:import namespace="c3a97ae1-1078-4f52-97c7-e1e75f184270"/>
@@ -3800,6 +3794,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{382CAFBC-27A9-4D0E-A532-4CEEC1A7F497}">
   <ds:schemaRefs>
@@ -3809,22 +3809,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6866972C-7532-44BD-9DE5-958311035541}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c3a97ae1-1078-4f52-97c7-e1e75f184270"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02023A10-1816-44FB-8F7C-8B09E93BD20F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3840,4 +3824,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6866972C-7532-44BD-9DE5-958311035541}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c3a97ae1-1078-4f52-97c7-e1e75f184270"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ADD train / factory begin system
</commit_message>
<xml_diff>
--- a/Documents/GameDesign/System_Design.xlsx
+++ b/Documents/GameDesign/System_Design.xlsx
@@ -8,35 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin DIJOUX\Documents\Unity\Workshop_TowerDefense\STD_Workshop\Documents\GameDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A5071B-57D3-42ED-B211-DBCBD7407770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354E58EA-8334-4259-9C22-D8986E8D1229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE4EEEAB-A39E-4793-9971-E358DB8AAF6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EE4EEEAB-A39E-4793-9971-E358DB8AAF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="TowerStatsCalc" sheetId="1" r:id="rId1"/>
-    <sheet name="Factory" sheetId="8" r:id="rId2"/>
-    <sheet name="Enemies" sheetId="3" r:id="rId3"/>
-    <sheet name="Tower" sheetId="4" r:id="rId4"/>
-    <sheet name="TowerUpdate" sheetId="7" r:id="rId5"/>
-    <sheet name="Weak" sheetId="5" r:id="rId6"/>
-    <sheet name="Data" sheetId="2" r:id="rId7"/>
+    <sheet name="Train" sheetId="9" r:id="rId2"/>
+    <sheet name="Factory" sheetId="8" r:id="rId3"/>
+    <sheet name="Enemies" sheetId="3" r:id="rId4"/>
+    <sheet name="Tower" sheetId="4" r:id="rId5"/>
+    <sheet name="TowerUpdate" sheetId="7" r:id="rId6"/>
+    <sheet name="Weak" sheetId="5" r:id="rId7"/>
+    <sheet name="Data" sheetId="2" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="CAT_ENEMIES">Data!$H$9:$H$11</definedName>
     <definedName name="CAT_TOWER">Data!$F$10:$F$12</definedName>
     <definedName name="CODE_ENEMIES">Enemies!$A$3:$A$11</definedName>
+    <definedName name="CODE_FACTORY">Factory!$A$3:$A$5</definedName>
     <definedName name="CODE_TOWER">Tower!$A$3:$A$11</definedName>
+    <definedName name="CODE_TRAIN">Train!$A$3:$A$5</definedName>
     <definedName name="CODE_UPGRADE">TowerUpdate!$A$3:$A$11</definedName>
     <definedName name="ENEMY">Enemies!$A$3:$H$11</definedName>
+    <definedName name="FACTORY">Factory!$A$3:$F$5</definedName>
     <definedName name="LEVEL_ENEMY">Data!$B$16:$B$21</definedName>
     <definedName name="SIGN">Data!$D$3:$D$6</definedName>
     <definedName name="STAT_ENEMY">Data!$H$3:$H$6</definedName>
+    <definedName name="STAT_FACTORY">Data!$L$3:$L$5</definedName>
     <definedName name="STAT_TOWER">Data!$F$3:$F$7</definedName>
     <definedName name="STAT_TRAIN">Data!$J$3:$J$5</definedName>
     <definedName name="STATS_TYPTOWER">Data!$B$24:$B$26</definedName>
     <definedName name="TOWER">Tower!$A$3:$I$11</definedName>
     <definedName name="TOWER_LVL2">Tower!$M$3:$Q$9</definedName>
     <definedName name="TOWER_UPGRADE">TowerUpdate!$A$3:$I$11</definedName>
+    <definedName name="TRAIN">Train!$A$3:$F$5</definedName>
     <definedName name="TYP_ENEMIES">Data!$H$14:$H$16</definedName>
     <definedName name="TYP_TOWER">Data!$F$15:$F$17</definedName>
     <definedName name="TYPE_TOWERELEMENT">Weak!$B$14:$B$22</definedName>
@@ -68,7 +74,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -90,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="162">
   <si>
     <t>Upgrade 1</t>
   </si>
@@ -534,6 +540,48 @@
   </si>
   <si>
     <t>Tower name</t>
+  </si>
+  <si>
+    <t>Bubblegum</t>
+  </si>
+  <si>
+    <t>Stars</t>
+  </si>
+  <si>
+    <t>STORAGE</t>
+  </si>
+  <si>
+    <t>SECONDS</t>
+  </si>
+  <si>
+    <t>Production / seconds</t>
+  </si>
+  <si>
+    <t>UNLOAD</t>
+  </si>
+  <si>
+    <t>Unload full to empty</t>
+  </si>
+  <si>
+    <t>²</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>Unload</t>
+  </si>
+  <si>
+    <t>Multiplicateur Factory</t>
+  </si>
+  <si>
+    <t>1_Piz</t>
+  </si>
+  <si>
+    <t>1_Car_Piz</t>
   </si>
 </sst>
 </file>
@@ -859,7 +907,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1056,161 +1104,199 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1219,7 +1305,7 @@
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
     <cellStyle name="Titre 3" xfId="2" builtinId="18"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="91">
     <dxf>
       <fill>
         <patternFill>
@@ -1363,14 +1449,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFF9999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1384,55 +1463,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1441,6 +1471,258 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1984,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDA4FAA-0409-4E65-B5DA-46DD5A6F91E2}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10:P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2016,41 +2298,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="115" t="s">
+      <c r="B1" s="113"/>
+      <c r="C1" s="98" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="13"/>
-      <c r="E1" s="115" t="s">
+      <c r="E1" s="98" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="13"/>
-      <c r="G1" s="115" t="s">
+      <c r="G1" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="101" t="s">
+      <c r="I1" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="101"/>
-      <c r="K1" s="103" t="s">
+      <c r="J1" s="110"/>
+      <c r="K1" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="103"/>
-      <c r="M1" s="101" t="s">
+      <c r="L1" s="107"/>
+      <c r="M1" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="101"/>
-      <c r="O1" s="103" t="s">
+      <c r="N1" s="110"/>
+      <c r="O1" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="103"/>
-      <c r="S1" s="103" t="s">
+      <c r="P1" s="107"/>
+      <c r="S1" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="103"/>
+      <c r="T1" s="107"/>
       <c r="U1" s="20"/>
       <c r="V1" s="20"/>
       <c r="W1" s="20"/>
@@ -2059,7 +2341,7 @@
       <c r="A2" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="99" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="11">
@@ -2080,33 +2362,33 @@
         <f t="array" ref="G2">_xlfn.IFS(F2="+",ROUNDDOWN(E2*(1+$I$2),2),F2="=",E2)</f>
         <v>6.76</v>
       </c>
-      <c r="I2" s="90">
+      <c r="I2" s="109">
         <v>0.3</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90">
+      <c r="J2" s="109"/>
+      <c r="K2" s="109">
         <v>0.2</v>
       </c>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90">
+      <c r="L2" s="109"/>
+      <c r="M2" s="109">
         <v>0.5</v>
       </c>
-      <c r="N2" s="90"/>
-      <c r="O2" s="73">
+      <c r="N2" s="109"/>
+      <c r="O2" s="108">
         <v>2</v>
       </c>
-      <c r="P2" s="73"/>
-      <c r="S2" s="72" t="s">
+      <c r="P2" s="108"/>
+      <c r="S2" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="72"/>
+      <c r="T2" s="105"/>
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
       <c r="W2" s="20"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="119"/>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="100" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="12">
@@ -2127,23 +2409,23 @@
         <f t="array" ref="G3">_xlfn.IFS(F3="+",ROUNDDOWN(E3*(1-$I$3),2),F3="=",E3)</f>
         <v>0.81</v>
       </c>
-      <c r="I3" s="102">
+      <c r="I3" s="111">
         <v>0.1</v>
       </c>
-      <c r="J3" s="102"/>
-      <c r="M3" s="102">
+      <c r="J3" s="111"/>
+      <c r="M3" s="111">
         <v>0.3</v>
       </c>
-      <c r="N3" s="102"/>
-      <c r="S3" s="72"/>
-      <c r="T3" s="72"/>
+      <c r="N3" s="111"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
       <c r="U3" s="20"/>
       <c r="V3" s="20"/>
       <c r="W3" s="20"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="119"/>
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="99" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="34">
@@ -2164,14 +2446,14 @@
         <f t="array" ref="G4">_xlfn.IFS(F4="+",ROUNDDOWN(E4*(1+$I$4),2),F4="=",E4)</f>
         <v>4.84</v>
       </c>
-      <c r="I4" s="90">
+      <c r="I4" s="109">
         <v>0.1</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="M4" s="90">
+      <c r="J4" s="109"/>
+      <c r="M4" s="109">
         <v>0.2</v>
       </c>
-      <c r="N4" s="90"/>
+      <c r="N4" s="109"/>
       <c r="T4" s="20"/>
       <c r="U4" s="20"/>
       <c r="V4" s="20"/>
@@ -2179,7 +2461,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="119"/>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="100" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="35">
@@ -2200,14 +2482,14 @@
         <f t="array" ref="G5">_xlfn.IFS(F5="+",ROUNDDOWN(E5*(1+$I$5),0),F5="=",E5)</f>
         <v>28</v>
       </c>
-      <c r="I5" s="102">
+      <c r="I5" s="111">
         <v>0.2</v>
       </c>
-      <c r="J5" s="102"/>
-      <c r="M5" s="102">
+      <c r="J5" s="111"/>
+      <c r="M5" s="111">
         <v>0.5</v>
       </c>
-      <c r="N5" s="102"/>
+      <c r="N5" s="111"/>
       <c r="T5" s="20"/>
       <c r="U5" s="20"/>
       <c r="V5" s="20"/>
@@ -2215,7 +2497,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="119"/>
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="99" t="s">
         <v>80</v>
       </c>
       <c r="C6" s="34">
@@ -2235,20 +2517,20 @@
         <f t="array" ref="G6">_xlfn.IFS(F6="+",ROUNDUP(E6*(1+$I$6),0),F6="=",E6)</f>
         <v>123</v>
       </c>
-      <c r="I6" s="90">
+      <c r="I6" s="109">
         <v>2.5</v>
       </c>
-      <c r="J6" s="90"/>
+      <c r="J6" s="109"/>
       <c r="T6" s="20"/>
       <c r="U6" s="20"/>
       <c r="V6" s="20"/>
       <c r="W6" s="20"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="113" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="118"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="64">
         <f>ROUNDDOWN(C2*C8,2)</f>
         <v>4</v>
@@ -2270,10 +2552,10 @@
       <c r="W7" s="20"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="112" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="122"/>
+      <c r="B8" s="112"/>
       <c r="C8" s="68">
         <f>1/C3</f>
         <v>1</v>
@@ -2296,74 +2578,74 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="O9" s="83" t="s">
+      <c r="O9" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="P9" s="83"/>
-      <c r="Q9" s="83" t="s">
+      <c r="P9" s="104"/>
+      <c r="Q9" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="R9" s="83"/>
-      <c r="S9" s="83" t="s">
+      <c r="R9" s="104"/>
+      <c r="S9" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="T9" s="83"/>
-      <c r="U9" s="83" t="s">
+      <c r="T9" s="104"/>
+      <c r="U9" s="104" t="s">
         <v>105</v>
       </c>
-      <c r="V9" s="83"/>
+      <c r="V9" s="104"/>
       <c r="W9" s="20"/>
     </row>
     <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="115" t="s">
+      <c r="C10" s="98" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="115" t="s">
+      <c r="E10" s="98" t="s">
         <v>69</v>
       </c>
       <c r="F10" s="13"/>
-      <c r="G10" s="115" t="s">
+      <c r="G10" s="98" t="s">
         <v>70</v>
       </c>
       <c r="H10" s="13"/>
-      <c r="I10" s="115" t="s">
+      <c r="I10" s="98" t="s">
         <v>71</v>
       </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="115" t="s">
+      <c r="K10" s="98" t="s">
         <v>72</v>
       </c>
       <c r="L10" s="13"/>
-      <c r="M10" s="115" t="s">
+      <c r="M10" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="72">
+      <c r="O10" s="105">
         <v>1</v>
       </c>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="107" t="str" cm="1">
+      <c r="P10" s="105"/>
+      <c r="Q10" s="106" t="str" cm="1">
         <f t="array" ref="Q10">_xlfn.IFS(O10=0, "=", O10&lt;&gt;0,HLOOKUP(Q9,UPGRADE_STAT,VLOOKUP(O14,UPGRADE_LVL,5,FALSE)+1,FALSE))</f>
         <v>+</v>
       </c>
-      <c r="R10" s="107"/>
-      <c r="S10" s="107" t="str" cm="1">
+      <c r="R10" s="106"/>
+      <c r="S10" s="106" t="str" cm="1">
         <f t="array" ref="S10">_xlfn.IFS(O10=0, "=", Q10&lt;&gt;0,HLOOKUP(S9,UPGRADE_STAT,VLOOKUP(O14,UPGRADE_LVL,5,FALSE)+1,FALSE))</f>
         <v>=</v>
       </c>
-      <c r="T10" s="107"/>
-      <c r="U10" s="107" t="str" cm="1">
+      <c r="T10" s="106"/>
+      <c r="U10" s="106" t="str" cm="1">
         <f t="array" ref="U10">_xlfn.IFS(O10=0, "=", S10&lt;&gt;0,HLOOKUP(U9,UPGRADE_STAT,VLOOKUP(O14,UPGRADE_LVL,5,FALSE)+1,FALSE))</f>
         <v>=</v>
       </c>
-      <c r="V10" s="107"/>
+      <c r="V10" s="106"/>
       <c r="W10" s="20"/>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="122"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="28">
         <f>G17</f>
         <v>6</v>
@@ -2403,8 +2685,8 @@
         <f t="array" ref="M11">_xlfn.IFS(L11="+",ROUNDDOWN(K11*(1+$M$2),2),L11="=",K11)</f>
         <v>45.55</v>
       </c>
-      <c r="O11" s="77"/>
-      <c r="P11" s="77"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="103"/>
       <c r="Q11" s="64"/>
       <c r="R11" s="64"/>
       <c r="S11" s="64"/>
@@ -2414,10 +2696,10 @@
       <c r="W11" s="20"/>
     </row>
     <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="118" t="s">
+      <c r="A12" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="118"/>
+      <c r="B12" s="113"/>
       <c r="C12" s="29">
         <f>I17</f>
         <v>5</v>
@@ -2463,10 +2745,10 @@
       <c r="W12" s="20"/>
     </row>
     <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="122"/>
+      <c r="B13" s="112"/>
       <c r="C13" s="28">
         <f>K17</f>
         <v>3</v>
@@ -2506,20 +2788,20 @@
         <f t="array" ref="M13">_xlfn.IFS(L13="+",ROUNDUP(K13*(1+$M$4),0),L13="=",K13)</f>
         <v>10</v>
       </c>
-      <c r="O13" s="116" t="s">
+      <c r="O13" s="102" t="s">
         <v>144</v>
       </c>
-      <c r="P13" s="116"/>
+      <c r="P13" s="102"/>
       <c r="T13" s="20"/>
       <c r="U13" s="20"/>
       <c r="V13" s="20"/>
       <c r="W13" s="20"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="118"/>
+      <c r="B14" s="113"/>
       <c r="C14" s="64">
         <f>M17</f>
         <v>2</v>
@@ -2559,11 +2841,11 @@
         <f t="array" ref="M14">_xlfn.IFS(L14="+",ROUNDUP(K14*(1+$M$5),0),L14="=",K14)</f>
         <v>18</v>
       </c>
-      <c r="O14" s="77" t="str">
+      <c r="O14" s="103" t="str">
         <f>_xlfn.CONCAT(C19," ",O10)</f>
         <v>Pizza 1</v>
       </c>
-      <c r="P14" s="77"/>
+      <c r="P14" s="103"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
@@ -2596,11 +2878,11 @@
       <c r="M16" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="O16" s="116" t="s">
+      <c r="O16" s="102" t="s">
         <v>147</v>
       </c>
-      <c r="P16" s="116"/>
-      <c r="Q16" s="116"/>
+      <c r="P16" s="102"/>
+      <c r="Q16" s="102"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
@@ -2636,12 +2918,12 @@
         <f>VLOOKUP($B$17,ENEMY,8)</f>
         <v>2</v>
       </c>
-      <c r="O17" s="124" t="str">
+      <c r="O17" s="101" t="str">
         <f>_xlfn.CONCAT(C19," ",E19," lvl ",O10)</f>
         <v>Pizza Mortar lvl 1</v>
       </c>
-      <c r="P17" s="124"/>
-      <c r="Q17" s="124"/>
+      <c r="P17" s="101"/>
+      <c r="Q17" s="101"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
@@ -2671,9 +2953,9 @@
       <c r="M18" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="O18" s="124"/>
-      <c r="P18" s="124"/>
-      <c r="Q18" s="124"/>
+      <c r="O18" s="101"/>
+      <c r="P18" s="101"/>
+      <c r="Q18" s="101"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
@@ -2711,40 +2993,40 @@
       </c>
     </row>
     <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="116" t="s">
+      <c r="B21" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="116"/>
-      <c r="E21" s="116" t="s">
+      <c r="C21" s="102"/>
+      <c r="E21" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="116"/>
-      <c r="G21" s="116"/>
-      <c r="H21" s="116"/>
-      <c r="I21" s="116"/>
-      <c r="K21" s="115" t="s">
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="102"/>
+      <c r="K21" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="M21" s="115" t="s">
+      <c r="M21" s="98" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="73">
+      <c r="B22" s="108">
         <f>ROUND(O2*K23*I23,2)</f>
         <v>8</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="E22" s="79" t="str">
+      <c r="C22" s="108"/>
+      <c r="E22" s="114" t="str">
         <f>C19</f>
         <v>Pizza</v>
       </c>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79" t="str">
+      <c r="F22" s="114"/>
+      <c r="G22" s="114" t="str">
         <f>C17</f>
         <v>Ghost</v>
       </c>
-      <c r="H22" s="79"/>
+      <c r="H22" s="114"/>
       <c r="I22" s="66" t="s">
         <v>39</v>
       </c>
@@ -2757,13 +3039,13 @@
       </c>
     </row>
     <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="80" t="str">
+      <c r="E23" s="118" t="str">
         <f>HLOOKUP(C19,WEAK_TOWER,VLOOKUP(C17,WEAK_ENEMY,5,FALSE)+1,FALSE)</f>
         <v>=</v>
       </c>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="80"/>
+      <c r="F23" s="118"/>
+      <c r="G23" s="118"/>
+      <c r="H23" s="118"/>
       <c r="I23" s="64" cm="1">
         <f t="array" ref="I23">_xlfn.IFS(E23="-", 1-K2, E23="=",1,E23="+",1+K2)</f>
         <v>1</v>
@@ -2781,27 +3063,27 @@
       <c r="T23" s="33"/>
     </row>
     <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="115" t="s">
+      <c r="K24" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="M24" s="115" t="s">
+      <c r="M24" s="98" t="s">
         <v>83</v>
       </c>
       <c r="Q24" s="32"/>
       <c r="R24" s="20"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C25" s="117" t="s">
+      <c r="C25" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="117"/>
-      <c r="E25" s="117"/>
-      <c r="F25" s="117"/>
-      <c r="G25" s="116" t="s">
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="H25" s="116"/>
-      <c r="I25" s="116"/>
+      <c r="H25" s="102"/>
+      <c r="I25" s="102"/>
       <c r="K25" s="64" cm="1">
         <f t="array" ref="K25">_xlfn.IFS(K22="Upgrade 0",C5,K22="Upgrade 1",E5,K22="Upgrade 2",G5)</f>
         <v>20</v>
@@ -2812,46 +3094,46 @@
       </c>
     </row>
     <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="116" t="s">
+      <c r="C26" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="116"/>
-      <c r="E26" s="116" t="s">
+      <c r="D26" s="102"/>
+      <c r="E26" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="116"/>
-      <c r="G26" s="77" t="str">
+      <c r="F26" s="102"/>
+      <c r="G26" s="103" t="str">
         <f>_xlfn.CONCAT(K25*K27," s")</f>
         <v>20 s</v>
       </c>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="K26" s="115" t="s">
+      <c r="H26" s="103"/>
+      <c r="I26" s="103"/>
+      <c r="K26" s="98" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="116" t="str">
+      <c r="B27" s="102" t="str">
         <f>_xlfn.CONCAT(K22," ",K21)</f>
         <v>Upgrade 0 DPS</v>
       </c>
-      <c r="C27" s="74">
+      <c r="C27" s="117">
         <f>ROUNDDOWN($M$23/B22,2)</f>
         <v>5.69</v>
       </c>
-      <c r="D27" s="74"/>
-      <c r="E27" s="75">
+      <c r="D27" s="117"/>
+      <c r="E27" s="116">
         <f>ROUNDUP($M$23/B22,0)</f>
         <v>6</v>
       </c>
-      <c r="F27" s="75"/>
-      <c r="G27" s="115" t="s">
+      <c r="F27" s="116"/>
+      <c r="G27" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="H27" s="116" t="s">
+      <c r="H27" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="I27" s="116"/>
+      <c r="I27" s="102"/>
       <c r="K27" s="64" cm="1">
         <f t="array" ref="K27">_xlfn.IFS(K22="Upgrade 0",C3,K22="Upgrade 1",E3,K22="Upgrade 2",G3)</f>
         <v>1</v>
@@ -2859,24 +3141,24 @@
       <c r="O27" s="18"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="116"/>
-      <c r="C28" s="77" t="str">
+      <c r="B28" s="102"/>
+      <c r="C28" s="103" t="str">
         <f>_xlfn.CONCAT(E27*K27," s")</f>
         <v>6 s</v>
       </c>
-      <c r="D28" s="77"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="77"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="103"/>
       <c r="G28" s="64">
         <f>E6+G6</f>
         <v>158</v>
       </c>
-      <c r="H28" s="77">
+      <c r="H28" s="103">
         <f>ROUNDUP(K29/M25,0)</f>
         <v>1</v>
       </c>
-      <c r="I28" s="77"/>
-      <c r="K28" s="115" t="s">
+      <c r="I28" s="103"/>
+      <c r="K28" s="98" t="s">
         <v>84</v>
       </c>
       <c r="N28" s="18"/>
@@ -2932,19 +3214,32 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="O17:Q18"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="E23:H23"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="S1:T1"/>
@@ -2961,32 +3256,19 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="O17:Q18"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C27">
@@ -3313,29 +3595,1043 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB692A4-AAE4-4AF5-8118-7C6BC2CF5B66}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D270C2D2-755B-49F6-BA6F-2E6401CF8C91}">
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="123" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="123"/>
+    <col min="1" max="1" width="14.28515625" style="45" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="45" customWidth="1"/>
+    <col min="3" max="6" width="11.42578125" style="45"/>
+    <col min="7" max="7" width="5.7109375" style="45" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="45"/>
+    <col min="10" max="10" width="5.7109375" style="45" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="45"/>
+    <col min="12" max="12" width="5.7109375" style="45" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="45"/>
+    <col min="14" max="14" width="5.7109375" style="45" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="45"/>
+    <col min="16" max="16" width="5.7109375" style="45" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="45"/>
+    <col min="18" max="18" width="5.7109375" style="45" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="45"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="59">
+        <v>1</v>
+      </c>
+      <c r="B1" s="59">
+        <v>2</v>
+      </c>
+      <c r="C1" s="59">
+        <v>3</v>
+      </c>
+      <c r="D1" s="59">
+        <v>4</v>
+      </c>
+      <c r="E1" s="59">
+        <v>5</v>
+      </c>
+      <c r="F1" s="59">
+        <v>6</v>
+      </c>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59">
+        <v>1</v>
+      </c>
+      <c r="I1" s="59">
+        <v>2</v>
+      </c>
+      <c r="J1" s="59">
+        <v>3</v>
+      </c>
+      <c r="K1" s="59">
+        <v>4</v>
+      </c>
+      <c r="L1" s="59">
+        <v>5</v>
+      </c>
+      <c r="M1" s="59">
+        <v>6</v>
+      </c>
+      <c r="N1" s="59">
+        <v>7</v>
+      </c>
+      <c r="O1" s="59">
+        <v>8</v>
+      </c>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+    </row>
+    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="73" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="76"/>
+      <c r="K2" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="76"/>
+      <c r="M2" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="76"/>
+      <c r="O2" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="89" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="str">
+        <f>_xlfn.CONCAT(B3,"_Car_",LEFT(C3,3))</f>
+        <v>1_Car_Piz</v>
+      </c>
+      <c r="B3" s="27">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="31">
+        <v>50</v>
+      </c>
+      <c r="E3" s="31">
+        <v>2</v>
+      </c>
+      <c r="F3" s="31">
+        <v>5</v>
+      </c>
+      <c r="H3" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" s="28">
+        <f>D3</f>
+        <v>50</v>
+      </c>
+      <c r="J3" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="28" cm="1">
+        <f t="array" ref="K3">_xlfn.IFS(J3="+",ROUNDUP($I$3 * (1 + Q3) ^ 1,0),J3="=",I3)</f>
+        <v>65</v>
+      </c>
+      <c r="L3" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="28" cm="1">
+        <f t="array" ref="M3">_xlfn.IFS(L3="+",ROUNDUP($I$3 * (1 + Q3) ^ 2,0),L3="=",K3)</f>
+        <v>65</v>
+      </c>
+      <c r="N3" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="28" cm="1">
+        <f t="array" ref="O3">_xlfn.IFS(N3="+",ROUNDUP($I$3 * (1 + Q3) ^ 3,0),N3="=",M3)</f>
+        <v>65</v>
+      </c>
+      <c r="Q3" s="83">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="90" t="str">
+        <f t="shared" ref="A4:A5" si="0">_xlfn.CONCAT(B4,"_Car_",LEFT(C4,3))</f>
+        <v>2_Car_Bub</v>
+      </c>
+      <c r="B4" s="27">
+        <v>2</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="29">
+        <f>D3</f>
+        <v>50</v>
+      </c>
+      <c r="E4" s="29">
+        <f t="shared" ref="E4" si="1">E3</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="29">
+        <f>F3</f>
+        <v>5</v>
+      </c>
+      <c r="H4" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="29">
+        <f>E3</f>
+        <v>2</v>
+      </c>
+      <c r="J4" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="29" cm="1">
+        <f t="array" ref="K4">_xlfn.IFS(J4="+",ROUNDDOWN($I$4 * (1 + Q4) ^ 1,2),J4="=",I4)</f>
+        <v>2</v>
+      </c>
+      <c r="L4" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="29" cm="1">
+        <f t="array" ref="M4">_xlfn.IFS(L4="+",ROUNDDOWN($I$4 * (1 + Q4) ^ 1,2),L4="=",I4)</f>
+        <v>2.6</v>
+      </c>
+      <c r="N4" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="29" cm="1">
+        <f t="array" ref="O4">_xlfn.IFS(N4="+",ROUNDDOWN($I$4 * (1 + Q4) ^ 3,2),N4="=",M4)</f>
+        <v>2.6</v>
+      </c>
+      <c r="Q4" s="90">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="83" t="str">
+        <f t="shared" si="0"/>
+        <v>3_Car_Sta</v>
+      </c>
+      <c r="B5" s="27">
+        <v>3</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="28">
+        <f>D3</f>
+        <v>50</v>
+      </c>
+      <c r="E5" s="28">
+        <f t="shared" ref="E5" si="2">E3</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="28">
+        <f>F3</f>
+        <v>5</v>
+      </c>
+      <c r="H5" s="78" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5" s="28">
+        <f>F3</f>
+        <v>5</v>
+      </c>
+      <c r="J5" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="28" cm="1">
+        <f t="array" ref="K5">_xlfn.IFS(J5="+",ROUNDDOWN($I$5 * (1 + Q5) ^ 1,2),J5="=",I5)</f>
+        <v>5</v>
+      </c>
+      <c r="L5" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="28" cm="1">
+        <f t="array" ref="M5">_xlfn.IFS(L5="+",ROUNDDOWN($I$5 * (1 + Q5) ^ 2,2),L5="=",K5)</f>
+        <v>5</v>
+      </c>
+      <c r="N5" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="28" cm="1">
+        <f t="array" ref="O5">_xlfn.IFS(N5="+",ROUNDUP($I$5 * (1 + Q5) ^ 1,0),N5="=",M5)</f>
+        <v>8</v>
+      </c>
+      <c r="Q5" s="83">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H6" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="29">
+        <v>10</v>
+      </c>
+      <c r="J6" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="29" cm="1">
+        <f t="array" ref="K6">_xlfn.IFS(J6="+",ROUNDUP($I$6 * (1 + Q6) ^ 1,2),J6="=",I6)</f>
+        <v>15</v>
+      </c>
+      <c r="L6" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="29" cm="1">
+        <f t="array" ref="M6">_xlfn.IFS(L6="+",ROUNDUP($I$6 * (1 + Q6) ^ 2,0),L6="=",I6)</f>
+        <v>23</v>
+      </c>
+      <c r="N6" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="29" cm="1">
+        <f t="array" ref="O6">_xlfn.IFS(N6="+",ROUNDUP($I$6 * (1 + Q6) ^ 3,0),N6="=",I6)</f>
+        <v>34</v>
+      </c>
+      <c r="Q6" s="90">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C7" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="120"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="121" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="121"/>
+      <c r="H8" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="82"/>
+      <c r="O8" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="77"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C9" s="121"/>
+      <c r="D9" s="121"/>
+      <c r="H9" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="I9" s="81" t="str">
+        <f>VLOOKUP($H$9,TRAIN,3)</f>
+        <v>Pizza</v>
+      </c>
+      <c r="J9" s="81"/>
+      <c r="K9" s="135">
+        <f>VLOOKUP($H$9,TRAIN,4)</f>
+        <v>50</v>
+      </c>
+      <c r="L9" s="81"/>
+      <c r="M9" s="135">
+        <f>VLOOKUP($H$9,TRAIN,5)</f>
+        <v>2</v>
+      </c>
+      <c r="N9" s="72"/>
+      <c r="O9" s="135">
+        <f>VLOOKUP($H$9,TRAIN,6)</f>
+        <v>5</v>
+      </c>
+      <c r="P9" s="72"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C10" s="136">
+        <f>D3/F3</f>
+        <v>10</v>
+      </c>
+      <c r="D10" s="136"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="C10:D10"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9" xr:uid="{4E0730DA-A975-4D36-89B9-EDD70882FA4F}">
+      <formula1>CODE_TRAIN</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J6 L3:L6 N3:N6 P3:P6 R3:R6" xr:uid="{3FA26D1C-C9BA-4446-AEF5-6139752B602A}">
+      <formula1>SIGN</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C5" xr:uid="{4BAA8DF3-38D8-473B-A9C1-B557BB4BC682}">
+      <formula1>STAT_FACTORY</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{2BC1FD63-8679-480D-8AFA-71B7EA976BD4}">
+            <xm:f>NOT(ISERROR(SEARCH("=",J3)))</xm:f>
+            <xm:f>"="</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J3:J6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{C4D66130-71E0-4188-9B0B-409EE70A7518}">
+            <xm:f>NOT(ISERROR(SEARCH("+",J3)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J3:J6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{172BB7CD-0792-4F79-95C9-2E47075AE0F8}">
+            <xm:f>NOT(ISERROR(SEARCH("=",L3)))</xm:f>
+            <xm:f>"="</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L3:L5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{214D66B2-1BE9-4903-96BA-A9F7040BC237}">
+            <xm:f>NOT(ISERROR(SEARCH("+",L3)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L3:L5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{E81E8F0D-C981-41E7-B507-33740C613E3B}">
+            <xm:f>NOT(ISERROR(SEARCH("=",N3)))</xm:f>
+            <xm:f>"="</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N3:N6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{EBC75F20-CF4A-4420-9B7B-B741E6F9218B}">
+            <xm:f>NOT(ISERROR(SEARCH("+",N3)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N3:N6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{BE721188-9C5A-4452-9BD3-D58EC020D450}">
+            <xm:f>NOT(ISERROR(SEARCH("=",L6)))</xm:f>
+            <xm:f>"="</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{D82E6B1C-3F48-4CE0-9B70-26B264E01C2C}">
+            <xm:f>NOT(ISERROR(SEARCH("+",L6)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L6</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB692A4-AAE4-4AF5-8118-7C6BC2CF5B66}">
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" style="45" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="45" customWidth="1"/>
+    <col min="3" max="6" width="11.42578125" style="45"/>
+    <col min="7" max="7" width="5.7109375" style="45" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="45"/>
+    <col min="10" max="10" width="5.7109375" style="45" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="45"/>
+    <col min="12" max="12" width="5.7109375" style="45" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="45"/>
+    <col min="14" max="14" width="5.7109375" style="45" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="45"/>
+    <col min="16" max="16" width="5.7109375" style="45" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="45"/>
+    <col min="18" max="18" width="5.7109375" style="45" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="45"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="59">
+        <v>1</v>
+      </c>
+      <c r="B1" s="59">
+        <v>2</v>
+      </c>
+      <c r="C1" s="59">
+        <v>3</v>
+      </c>
+      <c r="D1" s="59">
+        <v>4</v>
+      </c>
+      <c r="E1" s="59">
+        <v>5</v>
+      </c>
+      <c r="F1" s="59">
+        <v>6</v>
+      </c>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59">
+        <v>1</v>
+      </c>
+      <c r="I1" s="59">
+        <v>2</v>
+      </c>
+      <c r="J1" s="59">
+        <v>3</v>
+      </c>
+      <c r="K1" s="59">
+        <v>4</v>
+      </c>
+      <c r="L1" s="59">
+        <v>5</v>
+      </c>
+      <c r="M1" s="59">
+        <v>6</v>
+      </c>
+      <c r="N1" s="59">
+        <v>7</v>
+      </c>
+      <c r="O1" s="59">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="73" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="76"/>
+      <c r="K2" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="76"/>
+      <c r="M2" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="76"/>
+      <c r="O2" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="89" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="str">
+        <f>_xlfn.CONCAT(B3,"_",LEFT(C3,3))</f>
+        <v>1_Piz</v>
+      </c>
+      <c r="B3" s="27">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="31">
+        <v>100</v>
+      </c>
+      <c r="E3" s="31">
+        <v>2</v>
+      </c>
+      <c r="F3" s="31">
+        <v>10</v>
+      </c>
+      <c r="H3" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" s="28">
+        <f>D3</f>
+        <v>100</v>
+      </c>
+      <c r="J3" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="28" cm="1">
+        <f t="array" aca="1" ref="K3" ca="1">_xlfn.IFS(J3="+",ROUNDDOWN($K$3 * (1 + Q3) ^ 1,2),J3="=",I3)</f>
+        <v>15</v>
+      </c>
+      <c r="L3" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="28" cm="1">
+        <f t="array" ref="M3">_xlfn.IFS(L3="+",ROUNDDOWN($I$3 * (1 + Q3) ^ 2,2),L3="=",I3)</f>
+        <v>169</v>
+      </c>
+      <c r="N3" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="28" cm="1">
+        <f t="array" ref="O3">_xlfn.IFS(N3="+",ROUNDDOWN($I$3 * (1 + Q3) ^ 3,2),N3="=",I3)</f>
+        <v>219.7</v>
+      </c>
+      <c r="Q3" s="83">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="90" t="str">
+        <f t="shared" ref="A4:A5" si="0">_xlfn.CONCAT(B4,"_",LEFT(C4,3))</f>
+        <v>2_Bub</v>
+      </c>
+      <c r="B4" s="27">
+        <v>2</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="29">
+        <f>D3</f>
+        <v>100</v>
+      </c>
+      <c r="E4" s="29">
+        <f t="shared" ref="E4:G4" si="1">E3</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H4" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="29">
+        <f>E3</f>
+        <v>2</v>
+      </c>
+      <c r="J4" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="29" cm="1">
+        <f t="array" ref="K4">_xlfn.IFS(J4="+",ROUNDDOWN($I$4 * (1 + Q4) ^ 1,2),J4="=",I4)</f>
+        <v>2.6</v>
+      </c>
+      <c r="L4" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="29" cm="1">
+        <f t="array" ref="M4">_xlfn.IFS(L4="+",ROUNDDOWN($I$4 * (1 + Q4) ^ 2,2),L4="=",I4)</f>
+        <v>3.38</v>
+      </c>
+      <c r="N4" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="29" cm="1">
+        <f t="array" ref="O4">_xlfn.IFS(N4="+",ROUNDDOWN($I$4 * (1 + Q4) ^ 3,2),N4="=",I4)</f>
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="Q4" s="90">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="83" t="str">
+        <f t="shared" si="0"/>
+        <v>3_Sta</v>
+      </c>
+      <c r="B5" s="27">
+        <v>3</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="28">
+        <f>D3</f>
+        <v>100</v>
+      </c>
+      <c r="E5" s="28">
+        <f t="shared" ref="E5:G5" si="2">E3</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="28">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H5" s="78" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5" s="28">
+        <f>F3</f>
+        <v>10</v>
+      </c>
+      <c r="J5" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="28" cm="1">
+        <f t="array" aca="1" ref="K5" ca="1">_xlfn.IFS(J5="+",ROUNDDOWN($K$5 * (1 + Q5) ^ 1,2),J5="=",I5)</f>
+        <v>6</v>
+      </c>
+      <c r="L5" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="28" cm="1">
+        <f t="array" aca="1" ref="M5" ca="1">_xlfn.IFS(L5="+",ROUNDDOWN($K$5 * (1 + Q5) ^ 2,2),L5="=",I5)</f>
+        <v>7.2</v>
+      </c>
+      <c r="N5" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="28" cm="1">
+        <f t="array" aca="1" ref="O5" ca="1">_xlfn.IFS(N5="+",ROUNDDOWN($K$5 * (1 + Q5) ^ 3,2),N5="=",M5)</f>
+        <v>8.64</v>
+      </c>
+      <c r="Q5" s="83">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H6" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="29">
+        <v>10</v>
+      </c>
+      <c r="J6" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="29" cm="1">
+        <f t="array" ref="K6">_xlfn.IFS(J6="+",ROUNDUP($I$6 * (1 + Q6) ^ 1,2),J6="=",I6)</f>
+        <v>12</v>
+      </c>
+      <c r="L6" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="29" cm="1">
+        <f t="array" ref="M6">_xlfn.IFS(L6="+",ROUNDUP($I$6 * (1 + Q6) ^ 2,0),L6="=",I6)</f>
+        <v>15</v>
+      </c>
+      <c r="N6" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="29" cm="1">
+        <f t="array" ref="O6">_xlfn.IFS(N6="+",ROUNDUP($I$6 * (1 + Q6) ^ 3,0),N6="=",I6)</f>
+        <v>18</v>
+      </c>
+      <c r="Q6" s="90">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C7" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="120"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="121" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="121" t="s">
+        <v>154</v>
+      </c>
+      <c r="H8" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="82"/>
+      <c r="O8" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="77"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="121"/>
+      <c r="D9" s="121"/>
+      <c r="H9" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="I9" s="81" t="str">
+        <f>VLOOKUP($H$9,FACTORY,3)</f>
+        <v>Pizza</v>
+      </c>
+      <c r="J9" s="81"/>
+      <c r="K9" s="135">
+        <f>VLOOKUP($H$9,FACTORY,4)</f>
+        <v>100</v>
+      </c>
+      <c r="L9" s="81"/>
+      <c r="M9" s="135">
+        <f>VLOOKUP($H$9,FACTORY,5)</f>
+        <v>2</v>
+      </c>
+      <c r="N9" s="72"/>
+      <c r="O9" s="135">
+        <f>VLOOKUP($H$9,FACTORY,6)</f>
+        <v>10</v>
+      </c>
+      <c r="P9" s="72"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="28">
+        <f>ROUND(D3/E3,0)</f>
+        <v>50</v>
+      </c>
+      <c r="D10" s="28">
+        <f>D3/F3</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C5" xr:uid="{3B253C10-CDF1-4648-9DF4-6FC7222F90C3}">
+      <formula1>STAT_FACTORY</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J6 L3:L6 N3:N6 P3:P6 R3:R6" xr:uid="{521F7D0B-1CF3-43FC-9A6E-F52C923543F8}">
+      <formula1>SIGN</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9" xr:uid="{9822A667-ACA7-493D-8165-DFF96FA1B1AB}">
+      <formula1>CODE_FACTORY</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{2D7A5AC1-382C-4771-8D93-F63BA34D21A2}">
+            <xm:f>NOT(ISERROR(SEARCH("=",J3)))</xm:f>
+            <xm:f>"="</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J3:J6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{C62C2A07-5155-4334-93D2-0CA1FCC4355B}">
+            <xm:f>NOT(ISERROR(SEARCH("+",J3)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J3:J6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{D958A33F-9591-40E5-842E-45D140BCC588}">
+            <xm:f>NOT(ISERROR(SEARCH("=",L3)))</xm:f>
+            <xm:f>"="</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L3:L5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{00BC4EF5-3EDE-4EB2-99D8-E9171F2F5450}">
+            <xm:f>NOT(ISERROR(SEARCH("+",L3)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L3:L5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{70B003B0-A6DC-4880-82ED-30CFCAC64AD7}">
+            <xm:f>NOT(ISERROR(SEARCH("=",N3)))</xm:f>
+            <xm:f>"="</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N3:N6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{2D85DD62-DA29-4E5D-B4A6-EE0061934C18}">
+            <xm:f>NOT(ISERROR(SEARCH("+",N3)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N3:N6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{6A02CAD9-45B3-40E7-BD15-DB6C51024814}">
+            <xm:f>NOT(ISERROR(SEARCH("=",L6)))</xm:f>
+            <xm:f>"="</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{36AA0D63-ED68-478E-82B0-15A6C2683F1A}">
+            <xm:f>NOT(ISERROR(SEARCH("+",L6)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L6</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435E0B1E-C30D-4807-9C0B-B17E796108D4}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3595,36 +4891,36 @@
         <v>13</v>
       </c>
       <c r="M4" s="29" cm="1">
-        <f t="array" ref="M4">_xlfn.IFS(L4="+",ROUND($K$4 * (1 - W4) ^ 1,2),L4="=",K4)</f>
-        <v>2.1</v>
+        <f t="array" ref="M4">_xlfn.IFS(L4="+",ROUNDDOWN($K$4 * (1 + W4) ^ 1,2),L4="=",K4)</f>
+        <v>3.9</v>
       </c>
       <c r="N4" s="36" t="s">
         <v>13</v>
       </c>
       <c r="O4" s="29" cm="1">
-        <f t="array" ref="O4">_xlfn.IFS(L4="+",ROUND($K$4 * (1 - W4) ^ 2,2),L4="=",K4)</f>
-        <v>1.47</v>
+        <f t="array" ref="O4">_xlfn.IFS(N4="+",ROUNDDOWN($K$4 * (1 + W4) ^ 1,2),N4="=",M4)</f>
+        <v>3.9</v>
       </c>
       <c r="P4" s="36" t="s">
         <v>13</v>
       </c>
       <c r="Q4" s="29" cm="1">
-        <f t="array" ref="Q4">_xlfn.IFS(L4="+",ROUND($K$4 * (1 - W4) ^ 3,2),L4="=",K4)</f>
-        <v>1.03</v>
+        <f t="array" ref="Q4">_xlfn.IFS(P4="+",ROUNDDOWN($K$4 * (1 + W4) ^ 1,2),P4="=",O4)</f>
+        <v>3.9</v>
       </c>
       <c r="R4" s="36" t="s">
         <v>13</v>
       </c>
       <c r="S4" s="29" cm="1">
-        <f t="array" ref="S4">_xlfn.IFS(L4="+",ROUND($K$4 * (1 - W4) ^ 4,2),L4="=",K4)</f>
-        <v>0.72</v>
+        <f t="array" ref="S4">_xlfn.IFS(R4="+",ROUNDDOWN($K$4 * (1 + W4) ^ 1,2),R4="=",Q4)</f>
+        <v>3.9</v>
       </c>
       <c r="T4" s="36" t="s">
         <v>13</v>
       </c>
       <c r="U4" s="29" cm="1">
-        <f t="array" ref="U4">_xlfn.IFS(L4="+",ROUND($K$4 * (1 - W4) ^ 5,2),L4="=",K4)</f>
-        <v>0.5</v>
+        <f t="array" ref="U4">_xlfn.IFS(T4="+",ROUNDDOWN($K$4 * (1 + W4) ^ 1,2),T4="=",S4)</f>
+        <v>3.9</v>
       </c>
       <c r="V4" s="17"/>
       <c r="W4" s="14">
@@ -3845,18 +5141,18 @@
       <c r="J8" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="89" t="s">
+      <c r="K8" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89" t="s">
+      <c r="L8" s="82"/>
+      <c r="M8" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89" t="s">
+      <c r="N8" s="82"/>
+      <c r="O8" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="P8" s="89"/>
+      <c r="P8" s="82"/>
       <c r="Q8" s="26" t="s">
         <v>65</v>
       </c>
@@ -3902,16 +5198,16 @@
       <c r="J9" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="88" t="str">
+      <c r="K9" s="81" t="str">
         <f>VLOOKUP($J$9,ENEMY,3)</f>
         <v>Insect</v>
       </c>
-      <c r="L9" s="88"/>
-      <c r="M9" s="88" t="str">
+      <c r="L9" s="81"/>
+      <c r="M9" s="81" t="str">
         <f>VLOOKUP($J$9,ENEMY,4)</f>
         <v>Normal</v>
       </c>
-      <c r="N9" s="88"/>
+      <c r="N9" s="81"/>
       <c r="O9" s="68">
         <f>VLOOKUP($J$9,ENEMY,5)</f>
         <v>10</v>
@@ -3998,22 +5294,22 @@
       <c r="B12" s="60"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="120" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="76"/>
+      <c r="D13" s="120"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="121" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="D14" s="121" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C16" s="28">
@@ -4024,7 +5320,7 @@
         <f>G3/E3</f>
         <v>0.5</v>
       </c>
-      <c r="J16" s="87"/>
+      <c r="J16" s="80"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="29">
@@ -4220,12 +5516,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9045D55D-CDD5-4A2E-B7B4-999FBD02BF13}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4351,10 +5647,10 @@
       <c r="I2" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="K2" s="78" t="s">
+      <c r="K2" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="78"/>
+      <c r="L2" s="122"/>
       <c r="M2" s="42" t="s">
         <v>11</v>
       </c>
@@ -4384,7 +5680,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="str">
-        <f>_xlfn.CONCAT(B3,"_",LEFT(C3,4),"_",(LEFT(D3,4)))</f>
+        <f t="shared" ref="A3:A11" si="0">_xlfn.CONCAT(B3,"_",LEFT(C3,4),"_",(LEFT(D3,4)))</f>
         <v>1_Pizz_Snip</v>
       </c>
       <c r="B3" s="27">
@@ -4411,7 +5707,7 @@
       <c r="I3" s="31">
         <v>20</v>
       </c>
-      <c r="K3" s="81" t="s">
+      <c r="K3" s="125" t="s">
         <v>46</v>
       </c>
       <c r="L3" s="69" t="s">
@@ -4462,7 +5758,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="str">
-        <f>_xlfn.CONCAT(B4,"_",LEFT(C4,4),"_",(LEFT(D4,4)))</f>
+        <f t="shared" si="0"/>
         <v>2_Pizz_Mort</v>
       </c>
       <c r="B4" s="27">
@@ -4490,7 +5786,7 @@
         <f>I3</f>
         <v>20</v>
       </c>
-      <c r="K4" s="81"/>
+      <c r="K4" s="125"/>
       <c r="L4" s="70" t="s">
         <v>15</v>
       </c>
@@ -4539,7 +5835,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="str">
-        <f>_xlfn.CONCAT(B5,"_",LEFT(C5,4),"_",(LEFT(D5,4)))</f>
+        <f t="shared" si="0"/>
         <v>3_Pizz_Cano</v>
       </c>
       <c r="B5" s="27">
@@ -4567,7 +5863,7 @@
         <f>I3</f>
         <v>20</v>
       </c>
-      <c r="K5" s="81"/>
+      <c r="K5" s="125"/>
       <c r="L5" s="69" t="s">
         <v>10</v>
       </c>
@@ -4616,7 +5912,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="str">
-        <f>_xlfn.CONCAT(B6,"_",LEFT(C6,4),"_",(LEFT(D6,4)))</f>
+        <f t="shared" si="0"/>
         <v>4_Trap_Snip</v>
       </c>
       <c r="B6" s="27">
@@ -4648,7 +5944,7 @@
         <f>I3</f>
         <v>20</v>
       </c>
-      <c r="K6" s="81"/>
+      <c r="K6" s="125"/>
       <c r="L6" s="70" t="s">
         <v>41</v>
       </c>
@@ -4697,7 +5993,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="str">
-        <f>_xlfn.CONCAT(B7,"_",LEFT(C7,4),"_",(LEFT(D7,4)))</f>
+        <f t="shared" si="0"/>
         <v>5_Trap_Mort</v>
       </c>
       <c r="B7" s="27">
@@ -4710,26 +6006,26 @@
         <v>54</v>
       </c>
       <c r="E7" s="28">
-        <f>E4</f>
+        <f t="shared" ref="E7:H8" si="1">E4</f>
         <v>4</v>
       </c>
       <c r="F7" s="28">
-        <f>F4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G7" s="28">
-        <f>G4</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H7" s="28">
-        <f>H4</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I7" s="28">
         <f>I3</f>
         <v>20</v>
       </c>
-      <c r="K7" s="81"/>
+      <c r="K7" s="125"/>
       <c r="L7" s="69" t="s">
         <v>80</v>
       </c>
@@ -4777,7 +6073,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="str">
-        <f>_xlfn.CONCAT(B8,"_",LEFT(C8,4),"_",(LEFT(D8,4)))</f>
+        <f t="shared" si="0"/>
         <v>6_Trap_Cano</v>
       </c>
       <c r="B8" s="27">
@@ -4790,29 +6086,29 @@
         <v>53</v>
       </c>
       <c r="E8" s="29">
-        <f>E5</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="F8" s="29">
-        <f>F5</f>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="G8" s="29">
-        <f>G5</f>
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
       <c r="H8" s="29">
-        <f>H5</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="I8" s="29">
         <f>I3</f>
         <v>20</v>
       </c>
-      <c r="K8" s="84" t="s">
+      <c r="K8" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="L8" s="84"/>
+      <c r="L8" s="123"/>
       <c r="M8" s="41">
         <f>ROUNDDOWN(M3*M9,2)</f>
         <v>3.96</v>
@@ -4845,7 +6141,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="str">
-        <f>_xlfn.CONCAT(B9,"_",LEFT(C9,4),"_",(LEFT(D9,4)))</f>
+        <f t="shared" si="0"/>
         <v>7_Ener_Snip</v>
       </c>
       <c r="B9" s="27">
@@ -4877,10 +6173,10 @@
         <f>I3</f>
         <v>20</v>
       </c>
-      <c r="K9" s="85" t="s">
+      <c r="K9" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="85"/>
+      <c r="L9" s="124"/>
       <c r="M9" s="43">
         <f>ROUNDDOWN(1/M4,2)</f>
         <v>0.66</v>
@@ -4913,7 +6209,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="str">
-        <f>_xlfn.CONCAT(B10,"_",LEFT(C10,4),"_",(LEFT(D10,4)))</f>
+        <f t="shared" si="0"/>
         <v>8_Ener_Mort</v>
       </c>
       <c r="B10" s="27">
@@ -4926,19 +6222,19 @@
         <v>54</v>
       </c>
       <c r="E10" s="29">
-        <f>E4</f>
+        <f t="shared" ref="E10:H11" si="2">E4</f>
         <v>4</v>
       </c>
       <c r="F10" s="29">
-        <f>F4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G10" s="29">
-        <f>G4</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H10" s="29">
-        <f>H4</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I10" s="29">
@@ -4948,7 +6244,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="str">
-        <f>_xlfn.CONCAT(B11,"_",LEFT(C11,4),"_",(LEFT(D11,4)))</f>
+        <f t="shared" si="0"/>
         <v>9_Ener_Cano</v>
       </c>
       <c r="B11" s="27">
@@ -4961,116 +6257,116 @@
         <v>53</v>
       </c>
       <c r="E11" s="28">
-        <f>E5</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="F11" s="28">
-        <f>F5</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="G11" s="28">
-        <f>G5</f>
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
       <c r="H11" s="28">
-        <f>H5</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="I11" s="28">
         <f>I3</f>
         <v>20</v>
       </c>
-      <c r="K11" s="83" t="s">
+      <c r="K11" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83" t="s">
+      <c r="L11" s="104"/>
+      <c r="M11" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="83"/>
-      <c r="O11" s="83" t="s">
+      <c r="N11" s="104"/>
+      <c r="O11" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="P11" s="83"/>
-      <c r="Q11" s="83" t="s">
+      <c r="P11" s="104"/>
+      <c r="Q11" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="R11" s="83"/>
-      <c r="S11" s="83" t="s">
+      <c r="R11" s="104"/>
+      <c r="S11" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="T11" s="83"/>
-      <c r="U11" s="83" t="s">
+      <c r="T11" s="104"/>
+      <c r="U11" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="V11" s="83"/>
-      <c r="W11" s="83" t="s">
+      <c r="V11" s="104"/>
+      <c r="W11" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="X11" s="83"/>
-      <c r="Y11" s="83" t="s">
+      <c r="X11" s="104"/>
+      <c r="Y11" s="104" t="s">
         <v>96</v>
       </c>
-      <c r="Z11" s="83"/>
+      <c r="Z11" s="104"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K12" s="72" t="s">
+      <c r="K12" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="L12" s="72"/>
-      <c r="M12" s="73" t="str">
+      <c r="L12" s="105"/>
+      <c r="M12" s="108" t="str">
         <f>VLOOKUP($K$12,TOWER,3)</f>
         <v>Pizza</v>
       </c>
-      <c r="N12" s="73"/>
-      <c r="O12" s="73" t="str">
+      <c r="N12" s="108"/>
+      <c r="O12" s="108" t="str">
         <f>VLOOKUP($K$12,TOWER,4)</f>
         <v>Snipe</v>
       </c>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="73">
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108">
         <f>VLOOKUP($K$12,TOWER,5)</f>
         <v>6</v>
       </c>
-      <c r="R12" s="73"/>
-      <c r="S12" s="73">
+      <c r="R12" s="108"/>
+      <c r="S12" s="108">
         <f>VLOOKUP($K$12,TOWER,6)</f>
         <v>1.5</v>
       </c>
-      <c r="T12" s="73"/>
-      <c r="U12" s="73">
+      <c r="T12" s="108"/>
+      <c r="U12" s="108">
         <f>VLOOKUP($K$12,TOWER,7)</f>
         <v>5</v>
       </c>
-      <c r="V12" s="73"/>
-      <c r="W12" s="73">
+      <c r="V12" s="108"/>
+      <c r="W12" s="108">
         <f>VLOOKUP($K$12,TOWER,8)</f>
         <v>10</v>
       </c>
-      <c r="X12" s="73"/>
-      <c r="Y12" s="73">
+      <c r="X12" s="108"/>
+      <c r="Y12" s="108">
         <f>VLOOKUP($K$12,TOWER,9)</f>
         <v>20</v>
       </c>
-      <c r="Z12" s="73"/>
+      <c r="Z12" s="108"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="120" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="76"/>
+      <c r="D13" s="120"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="121" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="D14" s="121" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C16" s="28">
@@ -5104,13 +6400,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
     <mergeCell ref="W11:X11"/>
     <mergeCell ref="W12:X12"/>
     <mergeCell ref="Y11:Z11"/>
@@ -5127,6 +6416,13 @@
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C11" xr:uid="{A0725771-D6FB-4BCA-A3AB-AFBEDB867F7D}">
@@ -5184,7 +6480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356586D7-B694-445B-B036-FD29D6ACFCF6}">
   <dimension ref="A1:L15"/>
   <sheetViews>
@@ -5203,58 +6499,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="130" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="130" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="130" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="130" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="126" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="93"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="95" t="s">
+      <c r="H1" s="127"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="129" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="96" t="s">
+      <c r="A2" s="130"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="96" t="s">
+      <c r="H2" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="96" t="s">
+      <c r="I2" s="84" t="s">
         <v>105</v>
       </c>
-      <c r="J2" s="96" t="s">
+      <c r="J2" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="K2" s="96" t="s">
+      <c r="K2" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="L2" s="96" t="s">
+      <c r="L2" s="84" t="s">
         <v>108</v>
       </c>
     </row>
@@ -5275,16 +6571,16 @@
       <c r="E3" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="99" t="s">
+      <c r="F3" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="97" t="s">
+      <c r="G3" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="97" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="97" t="s">
+      <c r="H3" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="85" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="29"/>
@@ -5293,7 +6589,7 @@
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="str">
-        <f t="shared" ref="A4:A11" si="0">_xlfn.CONCAT(B4,"_",LEFT(C4,3), "_",D4)</f>
+        <f t="shared" ref="A4:A10" si="0">_xlfn.CONCAT(B4,"_",LEFT(C4,3), "_",D4)</f>
         <v>2_Tra_2a</v>
       </c>
       <c r="B4" s="28">
@@ -5308,16 +6604,16 @@
       <c r="E4" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="100" t="s">
+      <c r="F4" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="G4" s="98" t="s">
+      <c r="G4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="111" t="s">
+      <c r="H4" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="I4" s="98" t="s">
+      <c r="I4" s="86" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="28"/>
@@ -5341,16 +6637,16 @@
       <c r="E5" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="99" t="s">
+      <c r="F5" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="G5" s="97" t="s">
+      <c r="G5" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="112" t="s">
+      <c r="I5" s="96" t="s">
         <v>114</v>
       </c>
       <c r="J5" s="29"/>
@@ -5374,16 +6670,16 @@
       <c r="E6" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F6" s="100" t="s">
+      <c r="F6" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="G6" s="98" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="98" t="s">
+      <c r="G6" s="86" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="98" t="s">
+      <c r="I6" s="86" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="28"/>
@@ -5407,16 +6703,16 @@
       <c r="E7" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="F7" s="99" t="s">
+      <c r="F7" s="87" t="s">
         <v>120</v>
       </c>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="97" t="s">
+      <c r="H7" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="112" t="s">
+      <c r="I7" s="96" t="s">
         <v>114</v>
       </c>
       <c r="J7" s="29"/>
@@ -5440,16 +6736,16 @@
       <c r="E8" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="100" t="s">
+      <c r="F8" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="G8" s="111" t="s">
+      <c r="G8" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="H8" s="98" t="s">
+      <c r="H8" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="98" t="s">
+      <c r="I8" s="86" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="28"/>
@@ -5473,16 +6769,16 @@
       <c r="E9" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="F9" s="99" t="s">
+      <c r="F9" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="97" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="97" t="s">
+      <c r="G9" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="97" t="s">
+      <c r="I9" s="85" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="29"/>
@@ -5506,16 +6802,16 @@
       <c r="E10" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="100" t="s">
+      <c r="F10" s="88" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="98" t="s">
+      <c r="G10" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="H10" s="98" t="s">
+      <c r="H10" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="98" t="s">
+      <c r="I10" s="86" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="28"/>
@@ -5539,16 +6835,16 @@
       <c r="E11" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="F11" s="99" t="s">
+      <c r="F11" s="87" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="97" t="s">
+      <c r="G11" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="97" t="s">
+      <c r="H11" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="I11" s="97" t="s">
+      <c r="I11" s="85" t="s">
         <v>14</v>
       </c>
       <c r="J11" s="29"/>
@@ -5556,46 +6852,41 @@
       <c r="L11" s="29"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G13" s="89" t="s">
+      <c r="G13" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="89" t="s">
+      <c r="H13" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="89" t="s">
+      <c r="I13" s="82" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="105" t="s">
         <v>129</v>
       </c>
-      <c r="G14" s="73" t="str">
+      <c r="G14" s="108" t="str">
         <f>VLOOKUP($F$14,TOWER_UPGRADE,7)</f>
         <v>-</v>
       </c>
-      <c r="H14" s="73" t="str">
+      <c r="H14" s="108" t="str">
         <f>VLOOKUP($F$14,TOWER_UPGRADE,8)</f>
         <v>++</v>
       </c>
-      <c r="I14" s="73" t="str">
+      <c r="I14" s="108" t="str">
         <f>VLOOKUP($F$14,TOWER_UPGRADE,9)</f>
         <v>=</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F15" s="72"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="108"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -5603,6 +6894,11 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13 F14" xr:uid="{5DD3618D-C4BE-491F-B770-27363DACB01A}">
@@ -5667,7 +6963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483C23BD-B808-464E-B86B-8B4FE0CBBEE3}">
   <dimension ref="B2:P38"/>
   <sheetViews>
@@ -5732,11 +7028,11 @@
       <c r="F4" s="45">
         <v>2</v>
       </c>
-      <c r="G4" s="86" t="str">
+      <c r="G4" s="133" t="str">
         <f>HLOOKUP(G3,C2:E5,VLOOKUP(H3,B3:F5,5,FALSE)+1,FALSE)</f>
         <v>+</v>
       </c>
-      <c r="H4" s="86"/>
+      <c r="H4" s="133"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
@@ -5754,8 +7050,8 @@
       <c r="F5" s="45">
         <v>3</v>
       </c>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="46"/>
@@ -5808,11 +7104,11 @@
       <c r="F9" s="45">
         <v>2</v>
       </c>
-      <c r="G9" s="86" t="str">
+      <c r="G9" s="133" t="str">
         <f>HLOOKUP(G8,C7:E10,VLOOKUP(H8,B8:F10,5,FALSE)+1,FALSE)</f>
         <v>=</v>
       </c>
-      <c r="H9" s="86"/>
+      <c r="H9" s="133"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
@@ -5830,8 +7126,8 @@
       <c r="F10" s="45">
         <v>3</v>
       </c>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
       <c r="J10" s="4">
         <v>1</v>
       </c>
@@ -5846,11 +7142,11 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="106" t="s">
+      <c r="C12" s="132" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="132"/>
       <c r="J12" s="6">
         <f>COUNTIF(C14:E22,"=-")</f>
         <v>6</v>
@@ -5890,13 +7186,13 @@
       <c r="M13" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="O13" s="106" t="s">
+      <c r="O13" s="132" t="s">
         <v>141</v>
       </c>
-      <c r="P13" s="106"/>
+      <c r="P13" s="132"/>
     </row>
     <row r="14" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="91" t="s">
         <v>131</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -5917,19 +7213,19 @@
       <c r="H14" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J14" s="87">
+      <c r="J14" s="80">
         <f>COUNTIF(C14:E14,"=-")</f>
         <v>0</v>
       </c>
-      <c r="K14" s="87">
+      <c r="K14" s="80">
         <f>COUNTIF(C14:E14,"==")</f>
         <v>2</v>
       </c>
-      <c r="L14" s="87">
+      <c r="L14" s="80">
         <f>COUNTIF(C14:E14,"=+")</f>
         <v>1</v>
       </c>
-      <c r="M14" s="87">
+      <c r="M14" s="80">
         <f>COUNTIF(C14:E14,"=++")</f>
         <v>0</v>
       </c>
@@ -5937,13 +7233,13 @@
         <f>$J$10*J14+$K$10*K14+$L$10*L14+$M$10*M14</f>
         <v>7</v>
       </c>
-      <c r="P14" s="114">
+      <c r="P14" s="131">
         <f>ROUND(AVERAGE(O14:O22),0)</f>
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="92" t="s">
         <v>132</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -5958,24 +7254,24 @@
       <c r="F15" s="45">
         <v>2</v>
       </c>
-      <c r="G15" s="108" t="str">
+      <c r="G15" s="134" t="str">
         <f>HLOOKUP(G14,C13:E22,VLOOKUP(H14,B14:F22,5,FALSE)+1,FALSE)</f>
         <v>+</v>
       </c>
-      <c r="H15" s="108"/>
-      <c r="J15" s="87">
+      <c r="H15" s="134"/>
+      <c r="J15" s="80">
         <f t="shared" ref="J15:J22" si="0">COUNTIF(C15:E15,"=-")</f>
         <v>1</v>
       </c>
-      <c r="K15" s="87">
+      <c r="K15" s="80">
         <f t="shared" ref="K15:K22" si="1">COUNTIF(C15:E15,"==")</f>
         <v>1</v>
       </c>
-      <c r="L15" s="87">
+      <c r="L15" s="80">
         <f t="shared" ref="L15:L22" si="2">COUNTIF(C15:E15,"=+")</f>
         <v>0</v>
       </c>
-      <c r="M15" s="87">
+      <c r="M15" s="80">
         <f t="shared" ref="M15:M22" si="3">COUNTIF(C15:E15,"=++")</f>
         <v>1</v>
       </c>
@@ -5983,10 +7279,10 @@
         <f t="shared" ref="O15:O22" si="4">$J$10*J15+$K$10*K15+$L$10*L15+$M$10*M15</f>
         <v>7</v>
       </c>
-      <c r="P15" s="114"/>
+      <c r="P15" s="131"/>
     </row>
     <row r="16" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="91" t="s">
         <v>133</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -6001,21 +7297,21 @@
       <c r="F16" s="45">
         <v>3</v>
       </c>
-      <c r="G16" s="108"/>
-      <c r="H16" s="108"/>
-      <c r="J16" s="87">
+      <c r="G16" s="134"/>
+      <c r="H16" s="134"/>
+      <c r="J16" s="80">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K16" s="87">
+      <c r="K16" s="80">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L16" s="87">
+      <c r="L16" s="80">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M16" s="87">
+      <c r="M16" s="80">
         <f>COUNTIF(C16:E16,"=++")</f>
         <v>1</v>
       </c>
@@ -6023,10 +7319,10 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="P16" s="114"/>
+      <c r="P16" s="131"/>
     </row>
     <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="105" t="s">
+      <c r="B17" s="92" t="s">
         <v>134</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -6041,19 +7337,19 @@
       <c r="F17" s="45">
         <v>4</v>
       </c>
-      <c r="J17" s="87">
+      <c r="J17" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K17" s="87">
+      <c r="K17" s="80">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L17" s="87">
+      <c r="L17" s="80">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M17" s="87">
+      <c r="M17" s="80">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6061,10 +7357,10 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="P17" s="114"/>
+      <c r="P17" s="131"/>
     </row>
     <row r="18" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="91" t="s">
         <v>135</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -6079,19 +7375,19 @@
       <c r="F18" s="45">
         <v>5</v>
       </c>
-      <c r="J18" s="87">
+      <c r="J18" s="80">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K18" s="87">
+      <c r="K18" s="80">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L18" s="87">
+      <c r="L18" s="80">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M18" s="87">
+      <c r="M18" s="80">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -6099,13 +7395,13 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="P18" s="114"/>
+      <c r="P18" s="131"/>
     </row>
     <row r="19" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="105" t="s">
+      <c r="B19" s="92" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="109" t="s">
+      <c r="C19" s="93" t="s">
         <v>114</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -6117,19 +7413,19 @@
       <c r="F19" s="45">
         <v>6</v>
       </c>
-      <c r="J19" s="87">
+      <c r="J19" s="80">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K19" s="87">
+      <c r="K19" s="80">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L19" s="87">
+      <c r="L19" s="80">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M19" s="87">
+      <c r="M19" s="80">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -6137,10 +7433,10 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="P19" s="114"/>
+      <c r="P19" s="131"/>
     </row>
     <row r="20" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="91" t="s">
         <v>137</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -6155,19 +7451,19 @@
       <c r="F20" s="45">
         <v>7</v>
       </c>
-      <c r="J20" s="87">
+      <c r="J20" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="87">
+      <c r="K20" s="80">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L20" s="87">
+      <c r="L20" s="80">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M20" s="87">
+      <c r="M20" s="80">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6175,10 +7471,10 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="P20" s="114"/>
+      <c r="P20" s="131"/>
     </row>
     <row r="21" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="105" t="s">
+      <c r="B21" s="92" t="s">
         <v>138</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -6193,19 +7489,19 @@
       <c r="F21" s="45">
         <v>8</v>
       </c>
-      <c r="J21" s="87">
+      <c r="J21" s="80">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K21" s="87">
+      <c r="K21" s="80">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L21" s="87">
+      <c r="L21" s="80">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M21" s="87">
+      <c r="M21" s="80">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -6213,10 +7509,10 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="P21" s="114"/>
+      <c r="P21" s="131"/>
     </row>
     <row r="22" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="91" t="s">
         <v>139</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -6231,19 +7527,19 @@
       <c r="F22" s="45">
         <v>9</v>
       </c>
-      <c r="J22" s="87">
+      <c r="J22" s="80">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K22" s="87">
+      <c r="K22" s="80">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L22" s="87">
+      <c r="L22" s="80">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M22" s="87">
+      <c r="M22" s="80">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -6251,72 +7547,72 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="P22" s="114"/>
+      <c r="P22" s="131"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="104" t="s">
+      <c r="B24" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="87">
+      <c r="C24" s="80">
         <f>COUNTIF(C14:C22,"=-")</f>
         <v>3</v>
       </c>
-      <c r="D24" s="87">
+      <c r="D24" s="80">
         <f t="shared" ref="D24:E24" si="5">COUNTIF(D14:D22,"=-")</f>
         <v>2</v>
       </c>
-      <c r="E24" s="87">
+      <c r="E24" s="80">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="105" t="s">
+      <c r="B25" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="87">
+      <c r="C25" s="80">
         <f>COUNTIF(C14:C22,"==")</f>
         <v>2</v>
       </c>
-      <c r="D25" s="87">
+      <c r="D25" s="80">
         <f t="shared" ref="D25:E25" si="6">COUNTIF(D14:D22,"==")</f>
         <v>4</v>
       </c>
-      <c r="E25" s="87">
+      <c r="E25" s="80">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="104" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="87">
+      <c r="B26" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="80">
         <f>COUNTIF(C14:C22,"=+")</f>
         <v>2</v>
       </c>
-      <c r="D26" s="87">
+      <c r="D26" s="80">
         <f t="shared" ref="D26:E26" si="7">COUNTIF(D14:D22,"=+")</f>
         <v>1</v>
       </c>
-      <c r="E26" s="87">
+      <c r="E26" s="80">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="105" t="s">
+      <c r="B27" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="C27" s="87">
+      <c r="C27" s="80">
         <f>COUNTIF(C14:C22,"=++")</f>
         <v>2</v>
       </c>
-      <c r="D27" s="87">
+      <c r="D27" s="80">
         <f t="shared" ref="D27:E27" si="8">COUNTIF(D14:D22,"=++")</f>
         <v>2</v>
       </c>
-      <c r="E27" s="87">
+      <c r="E27" s="80">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
@@ -6336,51 +7632,51 @@
       </c>
     </row>
     <row r="30" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="114">
+      <c r="C30" s="131">
         <f>ROUND(AVERAGE(C29:E29),0)</f>
         <v>21</v>
       </c>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="131"/>
     </row>
     <row r="31" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="106" t="s">
+      <c r="C31" s="132" t="s">
         <v>141</v>
       </c>
-      <c r="D31" s="106"/>
-      <c r="E31" s="106"/>
+      <c r="D31" s="132"/>
+      <c r="E31" s="132"/>
     </row>
     <row r="32" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="113"/>
+      <c r="C32" s="97"/>
     </row>
     <row r="33" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="113"/>
+      <c r="C33" s="97"/>
     </row>
     <row r="34" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="113"/>
+      <c r="C34" s="97"/>
     </row>
     <row r="35" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="113"/>
+      <c r="C35" s="97"/>
     </row>
     <row r="36" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="113"/>
+      <c r="C36" s="97"/>
     </row>
     <row r="37" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="113"/>
+      <c r="C37" s="97"/>
     </row>
     <row r="38" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="113"/>
+      <c r="C38" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="P14:P22"/>
+    <mergeCell ref="O13:P13"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="G4:H5"/>
     <mergeCell ref="G9:H10"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="G15:H16"/>
-    <mergeCell ref="P14:P22"/>
-    <mergeCell ref="O13:P13"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:M22">
     <cfRule type="colorScale" priority="5">
@@ -6691,12 +7987,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B37B0DA-040C-4E1A-930F-48D7F5CF8BC3}">
-  <dimension ref="B1:J32"/>
+  <dimension ref="B1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6712,11 +8008,12 @@
     <col min="9" max="9" width="2.85546875" style="45" customWidth="1"/>
     <col min="10" max="10" width="21.42578125" style="45" customWidth="1"/>
     <col min="11" max="11" width="2.85546875" style="45" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="45"/>
+    <col min="12" max="12" width="21.42578125" style="45" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="47" t="s">
         <v>9</v>
       </c>
@@ -6732,13 +8029,16 @@
       <c r="J2" s="47" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="50"/>
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="94" t="s">
         <v>114</v>
       </c>
       <c r="E3" s="50"/>
@@ -6751,8 +8051,11 @@
       <c r="J3" s="52" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="49" t="s">
         <v>7</v>
       </c>
@@ -6770,8 +8073,11 @@
       <c r="J4" s="52" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="52" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="54" t="s">
         <v>8</v>
       </c>
@@ -6789,8 +8095,11 @@
       <c r="J5" s="56" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="56" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
       <c r="D6" s="55" t="s">
@@ -6804,7 +8113,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="48" t="s">
         <v>59</v>
       </c>
@@ -6814,7 +8123,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="51" t="s">
         <v>11</v>
       </c>
@@ -6825,7 +8134,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="49" t="s">
         <v>0</v>
       </c>
@@ -6836,7 +8145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="49" t="s">
         <v>2</v>
       </c>
@@ -6847,7 +8156,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="49" t="s">
         <v>1</v>
       </c>
@@ -6858,7 +8167,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="49" t="s">
         <v>3</v>
       </c>
@@ -6866,7 +8175,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="54" t="s">
         <v>4</v>
       </c>
@@ -6874,7 +8183,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="47" t="s">
         <v>56</v>
       </c>
@@ -6882,7 +8191,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="48" t="s">
         <v>75</v>
       </c>
@@ -6893,7 +8202,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="51" t="s">
         <v>68</v>
       </c>
@@ -6987,6 +8296,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100841444F490B10C45A279B0383115D26D" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="91c543cf6706f2108a45fe2b21185738">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c3a97ae1-1078-4f52-97c7-e1e75f184270" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6cf98f67490a83722a01f9dfd5fe46d6" ns3:_="">
     <xsd:import namespace="c3a97ae1-1078-4f52-97c7-e1e75f184270"/>
@@ -7118,35 +8442,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02023A10-1816-44FB-8F7C-8B09E93BD20F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{382CAFBC-27A9-4D0E-A532-4CEEC1A7F497}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c3a97ae1-1078-4f52-97c7-e1e75f184270"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7168,9 +8467,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{382CAFBC-27A9-4D0E-A532-4CEEC1A7F497}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02023A10-1816-44FB-8F7C-8B09E93BD20F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c3a97ae1-1078-4f52-97c7-e1e75f184270"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MODIFY System_Design.xlsx (Add Level 1) ADD Spider/Spider_Anim_V1.blend
ADD Test mesh scene in unity
</commit_message>
<xml_diff>
--- a/Documents/GameDesign/System_Design.xlsx
+++ b/Documents/GameDesign/System_Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GameSup_GD1\Workshop\Tower_Defense\STD_Workshop\Documents\GameDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486EE41F-4496-498D-9922-67C464538300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE107A02-1301-4EF3-99DE-7B97B78D6295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{EE4EEEAB-A39E-4793-9971-E358DB8AAF6E}"/>
   </bookViews>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="214">
   <si>
     <t>Upgrade 1</t>
   </si>
@@ -341,9 +341,6 @@
     <t>Full to Empty</t>
   </si>
   <si>
-    <t>Upgarde Cost</t>
-  </si>
-  <si>
     <t>$ Drop</t>
   </si>
   <si>
@@ -741,6 +738,9 @@
   </si>
   <si>
     <t>2_Car_Bub</t>
+  </si>
+  <si>
+    <t>Initial price</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1688,28 @@
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
     <cellStyle name="Titre 3" xfId="2" builtinId="18"/>
   </cellStyles>
-  <dxfs count="137">
+  <dxfs count="139">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDA2020"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDA2020"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1700,13 +1721,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDA2020"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3025,53 +3039,53 @@
     <row r="1" spans="1:48" s="111" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="108"/>
       <c r="B1" s="148" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1" s="140" t="s">
         <v>55</v>
       </c>
       <c r="D1" s="142" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E1" s="143"/>
       <c r="F1" s="144"/>
       <c r="G1" s="142" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H1" s="143"/>
       <c r="I1" s="144"/>
       <c r="J1" s="142" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K1" s="143"/>
       <c r="L1" s="144"/>
       <c r="M1" s="142" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N1" s="143"/>
       <c r="O1" s="144"/>
       <c r="P1" s="142" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q1" s="143"/>
       <c r="R1" s="144"/>
       <c r="S1" s="142" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T1" s="143"/>
       <c r="U1" s="144"/>
       <c r="V1" s="142" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="W1" s="143"/>
       <c r="X1" s="144"/>
       <c r="Y1" s="142" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z1" s="143"/>
       <c r="AA1" s="144"/>
       <c r="AB1" s="142" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AC1" s="143"/>
       <c r="AD1" s="144"/>
@@ -3099,58 +3113,58 @@
       <c r="B2" s="149"/>
       <c r="C2" s="141"/>
       <c r="D2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="G2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="I2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="H2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="I2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="J2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="K2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="L2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="K2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="L2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="M2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="N2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="O2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="N2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="O2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="P2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="R2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="Q2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="R2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="S2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="T2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="U2" s="126" t="s">
         <v>180</v>
-      </c>
-      <c r="T2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="U2" s="126" t="s">
-        <v>181</v>
       </c>
       <c r="V2" s="124"/>
       <c r="W2" s="125"/>
@@ -3173,7 +3187,7 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B3" s="99" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="104" t="str">
         <f t="shared" ref="C3:C11" si="0">VLOOKUP(B3,ENEMY,4)</f>
@@ -3236,7 +3250,7 @@
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B4" s="99" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="104" t="str">
         <f t="shared" si="0"/>
@@ -3299,7 +3313,7 @@
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B5" s="99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C5" s="104" t="str">
         <f t="shared" si="0"/>
@@ -3356,7 +3370,7 @@
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B6" s="99" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="104" t="str">
         <f t="shared" si="0"/>
@@ -3419,7 +3433,7 @@
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B7" s="99" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="104" t="str">
         <f t="shared" si="0"/>
@@ -3482,7 +3496,7 @@
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B8" s="99" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="104" t="str">
         <f t="shared" si="0"/>
@@ -3539,7 +3553,7 @@
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B9" s="99" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C9" s="104" t="str">
         <f t="shared" si="0"/>
@@ -3602,7 +3616,7 @@
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B10" s="99" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="104" t="str">
         <f t="shared" si="0"/>
@@ -3665,7 +3679,7 @@
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B11" s="99" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" s="104" t="str">
         <f t="shared" si="0"/>
@@ -3727,7 +3741,7 @@
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B13" s="82" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D13" s="145">
         <v>100</v>
@@ -3785,7 +3799,7 @@
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B14" s="86" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D14" s="131">
         <f>D3*VLOOKUP($B$3,ENEMY,7)+D4*VLOOKUP($B$4,ENEMY,7)+D5*VLOOKUP($B$5,ENEMY,7)+D6*VLOOKUP($B$6,ENEMY,7)+D7*VLOOKUP($B$7,ENEMY,7)+D8*VLOOKUP($B$8,ENEMY,7)+D9*VLOOKUP($B$9,ENEMY,7)+D10*VLOOKUP($B$10,ENEMY,7)+D11*VLOOKUP($B$11,ENEMY,7)</f>
@@ -3844,7 +3858,7 @@
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B15" s="86" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" s="131">
         <f>D25*VLOOKUP($B$25,TOWER,5)*VLOOKUP($B$25,TOWER,6)+D26*VLOOKUP($B$26,TOWER,5)*VLOOKUP($B$26,TOWER,6)+D27*VLOOKUP($B$27,TOWER,5)*VLOOKUP($B$27,TOWER,6)+D28*VLOOKUP($B$28,TOWER,5)*VLOOKUP($B$28,TOWER,6)+D29*VLOOKUP($B$29,TOWER,5)*VLOOKUP($B$29,TOWER,6)+D30*VLOOKUP($B$30,TOWER,5)*VLOOKUP($B$30,TOWER,6)+D31*VLOOKUP($B$31,TOWER,5)*VLOOKUP($B$31,TOWER,6)+D32*VLOOKUP($B$32,TOWER,5)*VLOOKUP($B$32,TOWER,6)+D33*VLOOKUP($B$33,TOWER,5)*VLOOKUP($B$33,TOWER,6)</f>
@@ -3903,7 +3917,7 @@
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B16" s="86" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D16" s="137">
         <f>D13-D14</f>
@@ -4001,41 +4015,41 @@
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B18" s="82" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D18" s="128">
         <f>Tower!I3*2+Tower!I3/2</f>
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="E18" s="129"/>
       <c r="F18" s="130"/>
       <c r="G18" s="128">
         <f>D21</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H18" s="129"/>
       <c r="I18" s="130"/>
       <c r="J18" s="128">
         <f t="shared" ref="J18" si="5">G21</f>
-        <v>12</v>
+        <v>-253</v>
       </c>
       <c r="K18" s="129"/>
       <c r="L18" s="130"/>
       <c r="M18" s="128">
         <f t="shared" ref="M18" si="6">J21</f>
-        <v>2</v>
+        <v>537</v>
       </c>
       <c r="N18" s="129"/>
       <c r="O18" s="130"/>
       <c r="P18" s="128">
         <f t="shared" ref="P18" si="7">M21</f>
-        <v>12</v>
+        <v>537</v>
       </c>
       <c r="Q18" s="129"/>
       <c r="R18" s="130"/>
       <c r="S18" s="128">
         <f t="shared" ref="S18" si="8">P21</f>
-        <v>12</v>
+        <v>2517</v>
       </c>
       <c r="T18" s="129"/>
       <c r="U18" s="130"/>
@@ -4060,41 +4074,41 @@
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B19" s="86" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D19" s="134">
         <f>D25*VLOOKUP($B$25,TOWER,9)+D26*VLOOKUP($B$26,TOWER,9)+D27*VLOOKUP($B$27,TOWER,9)+D28*VLOOKUP($B$28,TOWER,9)+D29*VLOOKUP($B$29,TOWER,9)+D30*VLOOKUP($B$30,TOWER,9)+D31*VLOOKUP($B$31,TOWER,9)+D32*VLOOKUP($B$32,TOWER,9)+D33*VLOOKUP($B$33,TOWER,9)</f>
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="E19" s="135"/>
       <c r="F19" s="136"/>
       <c r="G19" s="134">
         <f>G25*VLOOKUP($B$25,TOWER,9)+G26*VLOOKUP($B$26,TOWER,9)+G27*VLOOKUP($B$27,TOWER,9)+G28*VLOOKUP($B$28,TOWER,9)+G29*VLOOKUP($B$29,TOWER,9)+G30*VLOOKUP($B$30,TOWER,9)+G31*VLOOKUP($B$31,TOWER,9)+G32*VLOOKUP($B$32,TOWER,9)+G33*VLOOKUP($B$33,TOWER,9)</f>
-        <v>160</v>
+        <v>710</v>
       </c>
       <c r="H19" s="135"/>
       <c r="I19" s="136"/>
       <c r="J19" s="134">
         <f>J25*VLOOKUP($B$25,TOWER,9)+J26*VLOOKUP($B$26,TOWER,9)+J27*VLOOKUP($B$27,TOWER,9)+J28*VLOOKUP($B$28,TOWER,9)+J29*VLOOKUP($B$29,TOWER,9)+J30*VLOOKUP($B$30,TOWER,9)+J31*VLOOKUP($B$31,TOWER,9)+J32*VLOOKUP($B$32,TOWER,9)+J33*VLOOKUP($B$33,TOWER,9)</f>
-        <v>160</v>
+        <v>710</v>
       </c>
       <c r="K19" s="135"/>
       <c r="L19" s="136"/>
       <c r="M19" s="134">
         <f>M25*VLOOKUP($B$25,TOWER,9)+M26*VLOOKUP($B$26,TOWER,9)+M27*VLOOKUP($B$27,TOWER,9)+M28*VLOOKUP($B$28,TOWER,9)+M29*VLOOKUP($B$29,TOWER,9)+M30*VLOOKUP($B$30,TOWER,9)+M31*VLOOKUP($B$31,TOWER,9)+M32*VLOOKUP($B$32,TOWER,9)+M33*VLOOKUP($B$33,TOWER,9)</f>
-        <v>80</v>
+        <v>360</v>
       </c>
       <c r="N19" s="135"/>
       <c r="O19" s="136"/>
       <c r="P19" s="134">
         <f>P25*VLOOKUP($B$25,TOWER,9)+P26*VLOOKUP($B$26,TOWER,9)+P27*VLOOKUP($B$27,TOWER,9)+P28*VLOOKUP($B$28,TOWER,9)+P29*VLOOKUP($B$29,TOWER,9)+P30*VLOOKUP($B$30,TOWER,9)+P31*VLOOKUP($B$31,TOWER,9)+P32*VLOOKUP($B$32,TOWER,9)+P33*VLOOKUP($B$33,TOWER,9)</f>
-        <v>1080</v>
+        <v>4860</v>
       </c>
       <c r="Q19" s="135"/>
       <c r="R19" s="136"/>
       <c r="S19" s="134">
         <f>S25*VLOOKUP($B$25,TOWER,9)+S26*VLOOKUP($B$26,TOWER,9)+S27*VLOOKUP($B$27,TOWER,9)+S28*VLOOKUP($B$28,TOWER,9)+S29*VLOOKUP($B$29,TOWER,9)+S30*VLOOKUP($B$30,TOWER,9)+S31*VLOOKUP($B$31,TOWER,9)+S32*VLOOKUP($B$32,TOWER,9)+S33*VLOOKUP($B$33,TOWER,9)</f>
-        <v>5680</v>
+        <v>25560</v>
       </c>
       <c r="T19" s="135"/>
       <c r="U19" s="136"/>
@@ -4119,7 +4133,7 @@
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B20" s="86" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D20" s="128">
         <f>D3*VLOOKUP($B$3,ENEMY,8)+D4*VLOOKUP($B$4,ENEMY,8)+D5*VLOOKUP($B$5,ENEMY,8)+D6*VLOOKUP($B$6,ENEMY,8)+D7*VLOOKUP($B$7,ENEMY,8)+D8*VLOOKUP($B$8,ENEMY,8)+D9*VLOOKUP($B$9,ENEMY,8)+D10*VLOOKUP($B$10,ENEMY,8)+D11*VLOOKUP($B$11,ENEMY,8)</f>
@@ -4129,31 +4143,31 @@
       <c r="F20" s="130"/>
       <c r="G20" s="128">
         <f>G3*H3*VLOOKUP($B$3,ENEMY,8)+G4*H4*VLOOKUP($B$4,ENEMY,8)+G5*H5*VLOOKUP($B$5,ENEMY,8)+G6*H6*VLOOKUP($B$6,ENEMY,8)+G7*H7*VLOOKUP($B$7,ENEMY,8)+G8*H8*VLOOKUP($B$8,ENEMY,8)+G9*H9*VLOOKUP($B$9,ENEMY,8)+G10*H10*VLOOKUP($B$10,ENEMY,8)+G11*H11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>162</v>
+        <v>432</v>
       </c>
       <c r="H20" s="129"/>
       <c r="I20" s="130"/>
       <c r="J20" s="128">
         <f>J3*K3*VLOOKUP($B$3,ENEMY,8)+J4*K4*VLOOKUP($B$4,ENEMY,8)+J5*K5*VLOOKUP($B$5,ENEMY,8)+J6*K6*VLOOKUP($B$6,ENEMY,8)+J7*K7*VLOOKUP($B$7,ENEMY,8)+J8*K8*VLOOKUP($B$8,ENEMY,8)+J9*K9*VLOOKUP($B$9,ENEMY,8)+J10*K10*VLOOKUP($B$10,ENEMY,8)+J11*K11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>150</v>
+        <v>1500</v>
       </c>
       <c r="K20" s="129"/>
       <c r="L20" s="130"/>
       <c r="M20" s="128">
         <f>M3*N3*VLOOKUP($B$3,ENEMY,8)+M4*N4*VLOOKUP($B$4,ENEMY,8)+M5*N5*VLOOKUP($B$5,ENEMY,8)+M6*N6*VLOOKUP($B$6,ENEMY,8)+M7*N7*VLOOKUP($B$7,ENEMY,8)+M8*N8*VLOOKUP($B$8,ENEMY,8)+M9*N9*VLOOKUP($B$9,ENEMY,8)+M10*N10*VLOOKUP($B$10,ENEMY,8)+M11*N11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>90</v>
+        <v>360</v>
       </c>
       <c r="N20" s="129"/>
       <c r="O20" s="130"/>
       <c r="P20" s="128">
         <f>P3*Q3*VLOOKUP($B$3,ENEMY,8)+P4*Q4*VLOOKUP($B$4,ENEMY,8)+P5*Q5*VLOOKUP($B$5,ENEMY,8)+P6*Q6*VLOOKUP($B$6,ENEMY,8)+P7*Q7*VLOOKUP($B$7,ENEMY,8)+P8*Q8*VLOOKUP($B$8,ENEMY,8)+P9*Q9*VLOOKUP($B$9,ENEMY,8)+P10*Q10*VLOOKUP($B$10,ENEMY,8)+P11*Q11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>1080</v>
+        <v>6840</v>
       </c>
       <c r="Q20" s="129"/>
       <c r="R20" s="130"/>
       <c r="S20" s="128">
         <f>S3*T3*VLOOKUP($B$3,ENEMY,8)+S4*T4*VLOOKUP($B$4,ENEMY,8)+S5*T5*VLOOKUP($B$5,ENEMY,8)+S6*T6*VLOOKUP($B$6,ENEMY,8)+S7*T7*VLOOKUP($B$7,ENEMY,8)+S8*T8*VLOOKUP($B$8,ENEMY,8)+S9*T9*VLOOKUP($B$9,ENEMY,8)+S10*T10*VLOOKUP($B$10,ENEMY,8)+S11*T11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>6450</v>
+        <v>35700</v>
       </c>
       <c r="T20" s="129"/>
       <c r="U20" s="130"/>
@@ -4178,41 +4192,41 @@
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B21" s="86" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D21" s="134">
         <f>D18-D19+D20</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E21" s="135"/>
       <c r="F21" s="136"/>
       <c r="G21" s="134">
         <f>G18-G19+G20</f>
-        <v>12</v>
+        <v>-253</v>
       </c>
       <c r="H21" s="135"/>
       <c r="I21" s="136"/>
       <c r="J21" s="134">
         <f t="shared" ref="J21" si="9">J18-J19+J20</f>
-        <v>2</v>
+        <v>537</v>
       </c>
       <c r="K21" s="135"/>
       <c r="L21" s="136"/>
       <c r="M21" s="134">
         <f t="shared" ref="M21" si="10">M18-M19+M20</f>
-        <v>12</v>
+        <v>537</v>
       </c>
       <c r="N21" s="135"/>
       <c r="O21" s="136"/>
       <c r="P21" s="134">
         <f t="shared" ref="P21" si="11">P18-P19+P20</f>
-        <v>12</v>
+        <v>2517</v>
       </c>
       <c r="Q21" s="135"/>
       <c r="R21" s="136"/>
       <c r="S21" s="134">
         <f t="shared" ref="S21" si="12">S18-S19+S20</f>
-        <v>782</v>
+        <v>12657</v>
       </c>
       <c r="T21" s="135"/>
       <c r="U21" s="136"/>
@@ -4237,10 +4251,10 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B24" s="105" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24" s="106" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
@@ -4249,7 +4263,7 @@
         <v>40</v>
       </c>
       <c r="B25" s="99" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" s="100" t="str">
         <f t="shared" ref="C25:C33" si="13">VLOOKUP(B3,ENEMY,4)</f>
@@ -4308,7 +4322,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="107" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C26" s="100" t="str">
         <f t="shared" si="13"/>
@@ -4367,7 +4381,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="107" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C27" s="100" t="str">
         <f t="shared" si="13"/>
@@ -4426,7 +4440,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="99" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C28" s="100" t="str">
         <f t="shared" si="13"/>
@@ -4485,7 +4499,7 @@
         <v>40</v>
       </c>
       <c r="B29" s="107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C29" s="100" t="str">
         <f t="shared" si="13"/>
@@ -4542,7 +4556,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="107" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C30" s="100" t="str">
         <f t="shared" si="13"/>
@@ -4599,7 +4613,7 @@
         <v>40</v>
       </c>
       <c r="B31" s="99" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C31" s="100" t="str">
         <f t="shared" si="13"/>
@@ -4656,7 +4670,7 @@
         <v>40</v>
       </c>
       <c r="B32" s="107" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C32" s="100" t="str">
         <f t="shared" si="13"/>
@@ -4713,7 +4727,7 @@
         <v>40</v>
       </c>
       <c r="B33" s="107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="100" t="str">
         <f t="shared" si="13"/>
@@ -5180,7 +5194,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:AM21">
-    <cfRule type="cellIs" dxfId="136" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="138" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5201,8 +5215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECF5610-AFF3-4403-B872-F795309595A3}">
   <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19:AM19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5252,53 +5266,53 @@
     <row r="1" spans="1:48" s="111" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="108"/>
       <c r="B1" s="148" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1" s="140" t="s">
         <v>55</v>
       </c>
       <c r="D1" s="142" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E1" s="143"/>
       <c r="F1" s="144"/>
       <c r="G1" s="142" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H1" s="143"/>
       <c r="I1" s="144"/>
       <c r="J1" s="142" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K1" s="143"/>
       <c r="L1" s="144"/>
       <c r="M1" s="142" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N1" s="143"/>
       <c r="O1" s="144"/>
       <c r="P1" s="142" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q1" s="143"/>
       <c r="R1" s="144"/>
       <c r="S1" s="142" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T1" s="143"/>
       <c r="U1" s="144"/>
       <c r="V1" s="142" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="W1" s="143"/>
       <c r="X1" s="144"/>
       <c r="Y1" s="142" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z1" s="143"/>
       <c r="AA1" s="144"/>
       <c r="AB1" s="142" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AC1" s="143"/>
       <c r="AD1" s="144"/>
@@ -5326,85 +5340,85 @@
       <c r="B2" s="149"/>
       <c r="C2" s="141"/>
       <c r="D2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="G2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="I2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="H2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="I2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="J2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="K2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="L2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="K2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="L2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="M2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="N2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="O2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="N2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="O2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="P2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="R2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="Q2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="R2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="S2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="T2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="U2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="T2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="U2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="V2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="W2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="X2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="W2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="X2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="Y2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="Z2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="AA2" s="126" t="s">
-        <v>181</v>
-      </c>
       <c r="AB2" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="AC2" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD2" s="126" t="s">
         <v>180</v>
-      </c>
-      <c r="AC2" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD2" s="126" t="s">
-        <v>181</v>
       </c>
       <c r="AE2" s="124"/>
       <c r="AF2" s="125"/>
@@ -5418,7 +5432,7 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B3" s="180" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="104" t="str">
         <f t="shared" ref="C3:C11" si="0">VLOOKUP(B3,ENEMY,4)</f>
@@ -5430,15 +5444,33 @@
       <c r="G3" s="116"/>
       <c r="H3" s="94"/>
       <c r="I3" s="117"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="117"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="94"/>
-      <c r="R3" s="117"/>
+      <c r="J3" s="116">
+        <v>4</v>
+      </c>
+      <c r="K3" s="94">
+        <v>3</v>
+      </c>
+      <c r="L3" s="117">
+        <v>2</v>
+      </c>
+      <c r="M3" s="116">
+        <v>5</v>
+      </c>
+      <c r="N3" s="94">
+        <v>3</v>
+      </c>
+      <c r="O3" s="117">
+        <v>3</v>
+      </c>
+      <c r="P3" s="116">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="94">
+        <v>2</v>
+      </c>
+      <c r="R3" s="117">
+        <v>2</v>
+      </c>
       <c r="S3" s="116"/>
       <c r="T3" s="94"/>
       <c r="U3" s="117"/>
@@ -5463,7 +5495,7 @@
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B4" s="99" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="104" t="str">
         <f t="shared" si="0"/>
@@ -5508,7 +5540,7 @@
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B5" s="181" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C5" s="104" t="str">
         <f t="shared" si="0"/>
@@ -5553,7 +5585,7 @@
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B6" s="99" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="104" t="str">
         <f t="shared" si="0"/>
@@ -5598,7 +5630,7 @@
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B7" s="99" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="104" t="str">
         <f t="shared" si="0"/>
@@ -5643,7 +5675,7 @@
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B8" s="99" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="104" t="str">
         <f t="shared" si="0"/>
@@ -5688,7 +5720,7 @@
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B9" s="180" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C9" s="104" t="str">
         <f t="shared" si="0"/>
@@ -5701,20 +5733,32 @@
         <v>3</v>
       </c>
       <c r="H9" s="94">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I9" s="117">
         <v>2</v>
       </c>
-      <c r="J9" s="116"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="117"/>
+      <c r="J9" s="116">
+        <v>4</v>
+      </c>
+      <c r="K9" s="94">
+        <v>2</v>
+      </c>
+      <c r="L9" s="117">
+        <v>2</v>
+      </c>
       <c r="M9" s="116"/>
       <c r="N9" s="94"/>
       <c r="O9" s="117"/>
-      <c r="P9" s="116"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="117"/>
+      <c r="P9" s="116">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="94">
+        <v>1</v>
+      </c>
+      <c r="R9" s="117">
+        <v>2</v>
+      </c>
       <c r="S9" s="116"/>
       <c r="T9" s="94"/>
       <c r="U9" s="117"/>
@@ -5739,7 +5783,7 @@
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B10" s="99" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="104" t="str">
         <f t="shared" si="0"/>
@@ -5784,7 +5828,7 @@
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B11" s="181" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" s="104" t="str">
         <f t="shared" si="0"/>
@@ -5834,7 +5878,7 @@
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B13" s="95" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D13" s="145">
         <v>100</v>
@@ -5892,7 +5936,7 @@
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B14" s="97" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D14" s="131">
         <f>D3*VLOOKUP($B$3,ENEMY,7)+D4*VLOOKUP($B$4,ENEMY,7)+D5*VLOOKUP($B$5,ENEMY,7)+D6*VLOOKUP($B$6,ENEMY,7)+D7*VLOOKUP($B$7,ENEMY,7)+D8*VLOOKUP($B$8,ENEMY,7)+D9*VLOOKUP($B$9,ENEMY,7)+D10*VLOOKUP($B$10,ENEMY,7)+D11*VLOOKUP($B$11,ENEMY,7)</f>
@@ -5902,25 +5946,25 @@
       <c r="F14" s="133"/>
       <c r="G14" s="131">
         <f>G3*H3*VLOOKUP($B$3,ENEMY,7)+G4*H4*VLOOKUP($B$4,ENEMY,7)+G5*H5*VLOOKUP($B$5,ENEMY,7)+G6*H6*VLOOKUP($B$6,ENEMY,7)+G7*H7*VLOOKUP($B$7,ENEMY,7)+G8*H8*VLOOKUP($B$8,ENEMY,7)+G9*H9*VLOOKUP($B$9,ENEMY,7)+G10*H10*VLOOKUP($B$10,ENEMY,7)+G11*H11*VLOOKUP($B$11,ENEMY,7)</f>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H14" s="132"/>
       <c r="I14" s="133"/>
       <c r="J14" s="131">
         <f>J3*K3*VLOOKUP($B$3,ENEMY,7)+J4*K4*VLOOKUP($B$4,ENEMY,7)+J5*K5*VLOOKUP($B$5,ENEMY,7)+J6*K6*VLOOKUP($B$6,ENEMY,7)+J7*K7*VLOOKUP($B$7,ENEMY,7)+J8*K8*VLOOKUP($B$8,ENEMY,7)+J9*K9*VLOOKUP($B$9,ENEMY,7)+J10*K10*VLOOKUP($B$10,ENEMY,7)+J11*K11*VLOOKUP($B$11,ENEMY,7)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K14" s="132"/>
       <c r="L14" s="133"/>
       <c r="M14" s="131">
         <f>M3*N3*VLOOKUP($B$3,ENEMY,7)+M4*N4*VLOOKUP($B$4,ENEMY,7)+M5*N5*VLOOKUP($B$5,ENEMY,7)+M6*N6*VLOOKUP($B$6,ENEMY,7)+M7*N7*VLOOKUP($B$7,ENEMY,7)+M8*N8*VLOOKUP($B$8,ENEMY,7)+M9*N9*VLOOKUP($B$9,ENEMY,7)+M10*N10*VLOOKUP($B$10,ENEMY,7)+M11*N11*VLOOKUP($B$11,ENEMY,7)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="N14" s="132"/>
       <c r="O14" s="133"/>
       <c r="P14" s="131">
         <f>P3*Q3*VLOOKUP($B$3,ENEMY,7)+P4*Q4*VLOOKUP($B$4,ENEMY,7)+P5*Q5*VLOOKUP($B$5,ENEMY,7)+P6*Q6*VLOOKUP($B$6,ENEMY,7)+P7*Q7*VLOOKUP($B$7,ENEMY,7)+P8*Q8*VLOOKUP($B$8,ENEMY,7)+P9*Q9*VLOOKUP($B$9,ENEMY,7)+P10*Q10*VLOOKUP($B$10,ENEMY,7)+P11*Q11*VLOOKUP($B$11,ENEMY,7)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="Q14" s="132"/>
       <c r="R14" s="133"/>
@@ -5951,7 +5995,7 @@
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B15" s="97" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" s="131">
         <f>D26*VLOOKUP($B$26,TOWER,5)*VLOOKUP($B$26,TOWER,6)+D27*VLOOKUP($B$27,TOWER,5)*VLOOKUP($B$27,TOWER,6)+D28*VLOOKUP($B$28,TOWER,5)*VLOOKUP($B$28,TOWER,6)+D29*VLOOKUP($B$29,TOWER,5)*VLOOKUP($B$29,TOWER,6)+D30*VLOOKUP($B$30,TOWER,5)*VLOOKUP($B$30,TOWER,6)+D31*VLOOKUP($B$31,TOWER,5)*VLOOKUP($B$31,TOWER,6)+D32*VLOOKUP($B$32,TOWER,5)*VLOOKUP($B$32,TOWER,6)+D33*VLOOKUP($B$33,TOWER,5)*VLOOKUP($B$33,TOWER,6)+D34*VLOOKUP($B$34,TOWER,5)*VLOOKUP($B$34,TOWER,6)</f>
@@ -5967,19 +6011,19 @@
       <c r="I15" s="133"/>
       <c r="J15" s="131">
         <f>J26*VLOOKUP($B$26,TOWER,5)*VLOOKUP($B$26,TOWER,6)+J27*VLOOKUP($B$27,TOWER,5)*VLOOKUP($B$27,TOWER,6)+J28*VLOOKUP($B$28,TOWER,5)*VLOOKUP($B$28,TOWER,6)+J29*VLOOKUP($B$29,TOWER,5)*VLOOKUP($B$29,TOWER,6)+J30*VLOOKUP($B$30,TOWER,5)*VLOOKUP($B$30,TOWER,6)+J31*VLOOKUP($B$31,TOWER,5)*VLOOKUP($B$31,TOWER,6)+J32*VLOOKUP($B$32,TOWER,5)*VLOOKUP($B$32,TOWER,6)+J33*VLOOKUP($B$33,TOWER,5)*VLOOKUP($B$33,TOWER,6)+J34*VLOOKUP($B$34,TOWER,5)*VLOOKUP($B$34,TOWER,6)</f>
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="K15" s="132"/>
       <c r="L15" s="133"/>
       <c r="M15" s="131">
         <f>M26*VLOOKUP($B$26,TOWER,5)*VLOOKUP($B$26,TOWER,6)+M27*VLOOKUP($B$27,TOWER,5)*VLOOKUP($B$27,TOWER,6)+M28*VLOOKUP($B$28,TOWER,5)*VLOOKUP($B$28,TOWER,6)+M29*VLOOKUP($B$29,TOWER,5)*VLOOKUP($B$29,TOWER,6)+M30*VLOOKUP($B$30,TOWER,5)*VLOOKUP($B$30,TOWER,6)+M31*VLOOKUP($B$31,TOWER,5)*VLOOKUP($B$31,TOWER,6)+M32*VLOOKUP($B$32,TOWER,5)*VLOOKUP($B$32,TOWER,6)+M33*VLOOKUP($B$33,TOWER,5)*VLOOKUP($B$33,TOWER,6)+M34*VLOOKUP($B$34,TOWER,5)*VLOOKUP($B$34,TOWER,6)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N15" s="132"/>
       <c r="O15" s="133"/>
       <c r="P15" s="131">
         <f>P26*VLOOKUP($B$26,TOWER,5)*VLOOKUP($B$26,TOWER,6)+P27*VLOOKUP($B$27,TOWER,5)*VLOOKUP($B$27,TOWER,6)+P28*VLOOKUP($B$28,TOWER,5)*VLOOKUP($B$28,TOWER,6)+P29*VLOOKUP($B$29,TOWER,5)*VLOOKUP($B$29,TOWER,6)+P30*VLOOKUP($B$30,TOWER,5)*VLOOKUP($B$30,TOWER,6)+P31*VLOOKUP($B$31,TOWER,5)*VLOOKUP($B$31,TOWER,6)+P32*VLOOKUP($B$32,TOWER,5)*VLOOKUP($B$32,TOWER,6)+P33*VLOOKUP($B$33,TOWER,5)*VLOOKUP($B$33,TOWER,6)+P34*VLOOKUP($B$34,TOWER,5)*VLOOKUP($B$34,TOWER,6)</f>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="Q15" s="132"/>
       <c r="R15" s="133"/>
@@ -6010,7 +6054,7 @@
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B16" s="97" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D16" s="137">
         <f>D13-D14</f>
@@ -6108,88 +6152,88 @@
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B18" s="95" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D18" s="128">
         <f>Tower!I3*2+Tower!I3/2</f>
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="E18" s="129"/>
       <c r="F18" s="130"/>
       <c r="G18" s="128">
         <f>D22</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H18" s="129"/>
       <c r="I18" s="130"/>
       <c r="J18" s="128">
         <f t="shared" ref="J18" si="5">G22</f>
-        <v>-10</v>
+        <v>21</v>
       </c>
       <c r="K18" s="129"/>
       <c r="L18" s="130"/>
       <c r="M18" s="128">
         <f t="shared" ref="M18" si="6">J22</f>
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="N18" s="129"/>
       <c r="O18" s="130"/>
       <c r="P18" s="128">
         <f t="shared" ref="P18" si="7">M22</f>
-        <v>-10</v>
+        <v>-109</v>
       </c>
       <c r="Q18" s="129"/>
       <c r="R18" s="130"/>
       <c r="S18" s="128">
         <f t="shared" ref="S18" si="8">P22</f>
-        <v>-10</v>
+        <v>-89</v>
       </c>
       <c r="T18" s="129"/>
       <c r="U18" s="130"/>
       <c r="V18" s="128">
         <f t="shared" ref="V18" si="9">S22</f>
-        <v>-10</v>
+        <v>-89</v>
       </c>
       <c r="W18" s="129"/>
       <c r="X18" s="130"/>
       <c r="Y18" s="128">
         <f t="shared" ref="Y18" si="10">V22</f>
-        <v>-10</v>
+        <v>-89</v>
       </c>
       <c r="Z18" s="129"/>
       <c r="AA18" s="130"/>
       <c r="AB18" s="128">
         <f t="shared" ref="AB18" si="11">Y22</f>
-        <v>-10</v>
+        <v>-89</v>
       </c>
       <c r="AC18" s="129"/>
       <c r="AD18" s="130"/>
       <c r="AE18" s="128">
         <f t="shared" ref="AE18" si="12">AB22</f>
-        <v>-10</v>
+        <v>-89</v>
       </c>
       <c r="AF18" s="129"/>
       <c r="AG18" s="130"/>
       <c r="AH18" s="128">
         <f t="shared" ref="AH18" si="13">AE22</f>
-        <v>-10</v>
+        <v>-89</v>
       </c>
       <c r="AI18" s="129"/>
       <c r="AJ18" s="130"/>
       <c r="AK18" s="128">
         <f t="shared" ref="AK18" si="14">AH22</f>
-        <v>-10</v>
+        <v>-89</v>
       </c>
       <c r="AL18" s="129"/>
       <c r="AM18" s="130"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B19" s="97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D19" s="134">
         <f>D26*VLOOKUP($B$26,TOWER,9)+D27*VLOOKUP($B$27,TOWER,9)+D28*VLOOKUP($B$28,TOWER,9)+D29*VLOOKUP($B$29,TOWER,9)+D30*VLOOKUP($B$30,TOWER,9)+D31*VLOOKUP($B$31,TOWER,9)+D32*VLOOKUP($B$32,TOWER,9)+D33*VLOOKUP($B$33,TOWER,9)+D34*VLOOKUP($B$34,TOWER,9)</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="E19" s="135"/>
       <c r="F19" s="136"/>
@@ -6201,19 +6245,19 @@
       <c r="I19" s="136"/>
       <c r="J19" s="134">
         <f>J26*VLOOKUP($B$26,TOWER,9)+J27*VLOOKUP($B$27,TOWER,9)+J28*VLOOKUP($B$28,TOWER,9)+J29*VLOOKUP($B$29,TOWER,9)+J30*VLOOKUP($B$30,TOWER,9)+J31*VLOOKUP($B$31,TOWER,9)+J32*VLOOKUP($B$32,TOWER,9)+J33*VLOOKUP($B$33,TOWER,9)+J34*VLOOKUP($B$34,TOWER,9)</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="K19" s="135"/>
       <c r="L19" s="136"/>
       <c r="M19" s="134">
         <f>M26*VLOOKUP($B$26,TOWER,9)+M27*VLOOKUP($B$27,TOWER,9)+M28*VLOOKUP($B$28,TOWER,9)+M29*VLOOKUP($B$29,TOWER,9)+M30*VLOOKUP($B$30,TOWER,9)+M31*VLOOKUP($B$31,TOWER,9)+M32*VLOOKUP($B$32,TOWER,9)+M33*VLOOKUP($B$33,TOWER,9)+M34*VLOOKUP($B$34,TOWER,9)</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N19" s="135"/>
       <c r="O19" s="136"/>
       <c r="P19" s="134">
         <f>P26*VLOOKUP($B$26,TOWER,9)+P27*VLOOKUP($B$27,TOWER,9)+P28*VLOOKUP($B$28,TOWER,9)+P29*VLOOKUP($B$29,TOWER,9)+P30*VLOOKUP($B$30,TOWER,9)+P31*VLOOKUP($B$31,TOWER,9)+P32*VLOOKUP($B$32,TOWER,9)+P33*VLOOKUP($B$33,TOWER,9)+P34*VLOOKUP($B$34,TOWER,9)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q19" s="135"/>
       <c r="R19" s="136"/>
@@ -6262,17 +6306,17 @@
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B20" s="97" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D20" s="128">
         <f>SUM(HLOOKUP(E37,FSTATS,5,FALSE)*D37,HLOOKUP(E38,FSTATS,5,FALSE)*D38,HLOOKUP(E39,FSTATS,5,FALSE)*D39)</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="E20" s="129"/>
       <c r="F20" s="130"/>
       <c r="G20" s="128">
         <f>SUM(HLOOKUP(H37,FSTATS,5,FALSE)*G37,HLOOKUP(H38,FSTATS,5,FALSE)*G38,HLOOKUP(H39,FSTATS,5,FALSE)*G39)</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H20" s="129"/>
       <c r="I20" s="130"/>
@@ -6284,7 +6328,7 @@
       <c r="L20" s="130"/>
       <c r="M20" s="128">
         <f>SUM(HLOOKUP(N37,FSTATS,5,FALSE)*M37,HLOOKUP(N38,FSTATS,5,FALSE)*M38,HLOOKUP(N39,FSTATS,5,FALSE)*M39)</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="N20" s="129"/>
       <c r="O20" s="130"/>
@@ -6339,7 +6383,7 @@
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B21" s="97" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="134">
         <f>D3*VLOOKUP($B$3,ENEMY,8)+D4*VLOOKUP($B$4,ENEMY,8)+D5*VLOOKUP($B$5,ENEMY,8)+D6*VLOOKUP($B$6,ENEMY,8)+D7*VLOOKUP($B$7,ENEMY,8)+D8*VLOOKUP($B$8,ENEMY,8)+D9*VLOOKUP($B$9,ENEMY,8)+D10*VLOOKUP($B$10,ENEMY,8)+D11*VLOOKUP($B$11,ENEMY,8)</f>
@@ -6349,25 +6393,25 @@
       <c r="F21" s="136"/>
       <c r="G21" s="134">
         <f>G3*H3*VLOOKUP($B$3,ENEMY,8)+G4*H4*VLOOKUP($B$4,ENEMY,8)+G5*H5*VLOOKUP($B$5,ENEMY,8)+G6*H6*VLOOKUP($B$6,ENEMY,8)+G7*H7*VLOOKUP($B$7,ENEMY,8)+G8*H8*VLOOKUP($B$8,ENEMY,8)+G9*H9*VLOOKUP($B$9,ENEMY,8)+G10*H10*VLOOKUP($B$10,ENEMY,8)+G11*H11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="H21" s="135"/>
       <c r="I21" s="136"/>
       <c r="J21" s="134">
         <f>J3*K3*VLOOKUP($B$3,ENEMY,8)+J4*K4*VLOOKUP($B$4,ENEMY,8)+J5*K5*VLOOKUP($B$5,ENEMY,8)+J6*K6*VLOOKUP($B$6,ENEMY,8)+J7*K7*VLOOKUP($B$7,ENEMY,8)+J8*K8*VLOOKUP($B$8,ENEMY,8)+J9*K9*VLOOKUP($B$9,ENEMY,8)+J10*K10*VLOOKUP($B$10,ENEMY,8)+J11*K11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="K21" s="135"/>
       <c r="L21" s="136"/>
       <c r="M21" s="134">
         <f>M3*N3*VLOOKUP($B$3,ENEMY,8)+M4*N4*VLOOKUP($B$4,ENEMY,8)+M5*N5*VLOOKUP($B$5,ENEMY,8)+M6*N6*VLOOKUP($B$6,ENEMY,8)+M7*N7*VLOOKUP($B$7,ENEMY,8)+M8*N8*VLOOKUP($B$8,ENEMY,8)+M9*N9*VLOOKUP($B$9,ENEMY,8)+M10*N10*VLOOKUP($B$10,ENEMY,8)+M11*N11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="N21" s="135"/>
       <c r="O21" s="136"/>
       <c r="P21" s="134">
         <f>P3*Q3*VLOOKUP($B$3,ENEMY,8)+P4*Q4*VLOOKUP($B$4,ENEMY,8)+P5*Q5*VLOOKUP($B$5,ENEMY,8)+P6*Q6*VLOOKUP($B$6,ENEMY,8)+P7*Q7*VLOOKUP($B$7,ENEMY,8)+P8*Q8*VLOOKUP($B$8,ENEMY,8)+P9*Q9*VLOOKUP($B$9,ENEMY,8)+P10*Q10*VLOOKUP($B$10,ENEMY,8)+P11*Q11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="Q21" s="135"/>
       <c r="R21" s="136"/>
@@ -6416,87 +6460,87 @@
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B22" s="97" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D22" s="128">
         <f>D18-(D19+D20)+D21</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E22" s="129"/>
       <c r="F22" s="130"/>
       <c r="G22" s="128">
-        <f>G18-(G19+G20)</f>
-        <v>-10</v>
+        <f>G18-(G19+G20)+G21</f>
+        <v>21</v>
       </c>
       <c r="H22" s="129"/>
       <c r="I22" s="130"/>
       <c r="J22" s="128">
-        <f t="shared" ref="J22:AM22" si="15">J18-(J19+J20)</f>
-        <v>-10</v>
+        <f t="shared" ref="J22" si="15">J18-(J19+J20)+J21</f>
+        <v>1</v>
       </c>
       <c r="K22" s="129"/>
       <c r="L22" s="130"/>
       <c r="M22" s="128">
-        <f t="shared" ref="M22:AM22" si="16">M18-(M19+M20)</f>
-        <v>-10</v>
+        <f t="shared" ref="M22" si="16">M18-(M19+M20)+M21</f>
+        <v>-109</v>
       </c>
       <c r="N22" s="129"/>
       <c r="O22" s="130"/>
       <c r="P22" s="128">
-        <f t="shared" ref="P22:AM22" si="17">P18-(P19+P20)</f>
-        <v>-10</v>
+        <f t="shared" ref="P22" si="17">P18-(P19+P20)+P21</f>
+        <v>-89</v>
       </c>
       <c r="Q22" s="129"/>
       <c r="R22" s="130"/>
       <c r="S22" s="128">
-        <f t="shared" ref="S22:AM22" si="18">S18-(S19+S20)</f>
-        <v>-10</v>
+        <f t="shared" ref="S22" si="18">S18-(S19+S20)+S21</f>
+        <v>-89</v>
       </c>
       <c r="T22" s="129"/>
       <c r="U22" s="130"/>
       <c r="V22" s="128">
-        <f t="shared" ref="V22:AM22" si="19">V18-(V19+V20)</f>
-        <v>-10</v>
+        <f t="shared" ref="V22" si="19">V18-(V19+V20)+V21</f>
+        <v>-89</v>
       </c>
       <c r="W22" s="129"/>
       <c r="X22" s="130"/>
       <c r="Y22" s="128">
-        <f t="shared" ref="Y22:AM22" si="20">Y18-(Y19+Y20)</f>
-        <v>-10</v>
+        <f t="shared" ref="Y22" si="20">Y18-(Y19+Y20)+Y21</f>
+        <v>-89</v>
       </c>
       <c r="Z22" s="129"/>
       <c r="AA22" s="130"/>
       <c r="AB22" s="128">
-        <f t="shared" ref="AB22:AM22" si="21">AB18-(AB19+AB20)</f>
-        <v>-10</v>
+        <f t="shared" ref="AB22" si="21">AB18-(AB19+AB20)+AB21</f>
+        <v>-89</v>
       </c>
       <c r="AC22" s="129"/>
       <c r="AD22" s="130"/>
       <c r="AE22" s="128">
-        <f t="shared" ref="AE22:AM22" si="22">AE18-(AE19+AE20)</f>
-        <v>-10</v>
+        <f t="shared" ref="AE22" si="22">AE18-(AE19+AE20)+AE21</f>
+        <v>-89</v>
       </c>
       <c r="AF22" s="129"/>
       <c r="AG22" s="130"/>
       <c r="AH22" s="128">
-        <f t="shared" ref="AH22:AM22" si="23">AH18-(AH19+AH20)</f>
-        <v>-10</v>
+        <f t="shared" ref="AH22" si="23">AH18-(AH19+AH20)+AH21</f>
+        <v>-89</v>
       </c>
       <c r="AI22" s="129"/>
       <c r="AJ22" s="130"/>
       <c r="AK22" s="128">
-        <f t="shared" ref="AK22:AM22" si="24">AK18-(AK19+AK20)</f>
-        <v>-10</v>
+        <f t="shared" ref="AK22" si="24">AK18-(AK19+AK20)+AK21</f>
+        <v>-89</v>
       </c>
       <c r="AL22" s="129"/>
       <c r="AM22" s="130"/>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B25" s="105" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" s="106" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
@@ -6505,7 +6549,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="99" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C26" s="100" t="str">
         <f>VLOOKUP(B3,ENEMY,4)</f>
@@ -6554,7 +6598,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="107" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C27" s="100" t="str">
         <f>VLOOKUP(B4,ENEMY,4)</f>
@@ -6600,10 +6644,10 @@
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="109">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B28" s="107" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C28" s="100" t="str">
         <f>VLOOKUP(B5,ENEMY,4)</f>
@@ -6619,13 +6663,19 @@
       <c r="G28" s="184"/>
       <c r="H28" s="129"/>
       <c r="I28" s="130"/>
-      <c r="J28" s="184"/>
-      <c r="K28" s="129"/>
+      <c r="J28" s="184">
+        <v>1</v>
+      </c>
+      <c r="K28" s="129" t="s">
+        <v>67</v>
+      </c>
       <c r="L28" s="130"/>
       <c r="M28" s="184"/>
       <c r="N28" s="129"/>
       <c r="O28" s="130"/>
-      <c r="P28" s="184"/>
+      <c r="P28" s="184">
+        <v>1</v>
+      </c>
       <c r="Q28" s="129"/>
       <c r="R28" s="130"/>
       <c r="S28" s="184"/>
@@ -6656,7 +6706,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="99" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C29" s="100" t="str">
         <f>VLOOKUP(B6,ENEMY,4)</f>
@@ -6702,10 +6752,10 @@
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="109">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B30" s="107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C30" s="100" t="str">
         <f>VLOOKUP(B7,ENEMY,4)</f>
@@ -6717,11 +6767,19 @@
       <c r="G30" s="184"/>
       <c r="H30" s="129"/>
       <c r="I30" s="130"/>
-      <c r="J30" s="184"/>
-      <c r="K30" s="129"/>
+      <c r="J30" s="184">
+        <v>1</v>
+      </c>
+      <c r="K30" s="129" t="s">
+        <v>66</v>
+      </c>
       <c r="L30" s="130"/>
-      <c r="M30" s="184"/>
-      <c r="N30" s="129"/>
+      <c r="M30" s="184">
+        <v>1</v>
+      </c>
+      <c r="N30" s="129" t="s">
+        <v>67</v>
+      </c>
       <c r="O30" s="130"/>
       <c r="P30" s="184"/>
       <c r="Q30" s="129"/>
@@ -6754,7 +6812,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="107" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C31" s="100" t="str">
         <f>VLOOKUP(B8,ENEMY,4)</f>
@@ -6803,7 +6861,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="99" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C32" s="100" t="str">
         <f>VLOOKUP(B9,ENEMY,4)</f>
@@ -6852,7 +6910,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="107" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C33" s="100" t="str">
         <f>VLOOKUP(B10,ENEMY,4)</f>
@@ -6901,7 +6959,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" s="100" t="str">
         <f>VLOOKUP(B11,ENEMY,4)</f>
@@ -6974,10 +7032,10 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B36" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="C36" s="105" t="s">
         <v>210</v>
-      </c>
-      <c r="C36" s="105" t="s">
-        <v>211</v>
       </c>
       <c r="D36" s="110"/>
       <c r="F36" s="31"/>
@@ -7083,7 +7141,7 @@
     <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="109">
         <f>SUM(D38:BA38)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B38" s="182" t="str">
         <f>Factory!A4</f>
@@ -7110,9 +7168,11 @@
         <v>66</v>
       </c>
       <c r="L38" s="130"/>
-      <c r="M38" s="184"/>
+      <c r="M38" s="184">
+        <v>1</v>
+      </c>
       <c r="N38" s="129" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O38" s="130"/>
       <c r="P38" s="184"/>
@@ -7513,6 +7573,18 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:AM16">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFFEB84"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:AM13">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -7524,20 +7596,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G13:AM13">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="100"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color rgb="FFFFEB84"/>
-        <color theme="9" tint="0.39997558519241921"/>
-      </colorScale>
+  <conditionalFormatting sqref="G22:AM22">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G22:AM22">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="D22:AM22">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7636,17 +7701,17 @@
       </c>
       <c r="P1" s="146"/>
       <c r="Q1" s="159" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R1" s="159"/>
       <c r="S1" s="159" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T1" s="159"/>
       <c r="U1" s="16"/>
       <c r="V1" s="16"/>
       <c r="W1" s="146" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X1" s="146"/>
     </row>
@@ -7806,21 +7871,21 @@
       </c>
       <c r="C5" s="25">
         <f>$X$33</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D5" s="75" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="25" cm="1">
         <f t="array" ref="E5">_xlfn.IFS(D5="+",ROUNDDOWN(C5*(1+$I$5),0),D5="=",C5)</f>
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="F5" s="75" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="25" cm="1">
         <f t="array" ref="G5">_xlfn.IFS(F5="+",ROUNDDOWN(E5*(1+$I$5),0),F5="=",E5)</f>
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="I5" s="153">
         <v>0.2</v>
@@ -7949,7 +8014,7 @@
         <v>71</v>
       </c>
       <c r="O9" s="155" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P9" s="155"/>
       <c r="Q9" s="155" t="s">
@@ -7957,11 +8022,11 @@
       </c>
       <c r="R9" s="155"/>
       <c r="S9" s="155" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T9" s="155"/>
       <c r="U9" s="155" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V9" s="155"/>
       <c r="W9" s="16"/>
@@ -8001,7 +8066,7 @@
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="150" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B11" s="76" t="s">
         <v>28</v>
@@ -8160,42 +8225,42 @@
       </c>
       <c r="C14" s="48">
         <f>X31</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D14" s="75" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="21" cm="1">
         <f t="array" ref="E14">_xlfn.IFS(D14="+",ROUNDUP(C14*(1+$M$5),0),D14="=",C14)</f>
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F14" s="75" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="21" cm="1">
         <f t="array" ref="G14">_xlfn.IFS(F14="+",ROUNDUP(E14*(1+$M$5),0),F14="=",E14)</f>
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="H14" s="75" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="21" cm="1">
         <f t="array" ref="I14">_xlfn.IFS(H14="+",ROUNDUP(G14*(1+$M$5),0),H14="=",G14)</f>
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="J14" s="75" t="s">
         <v>13</v>
       </c>
       <c r="K14" s="21" cm="1">
         <f t="array" ref="K14">_xlfn.IFS(J14="+",ROUNDUP(I14*(1+$M$5),0),J14="=",I14)</f>
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="L14" s="75" t="s">
         <v>13</v>
       </c>
       <c r="M14" s="21" cm="1">
         <f t="array" ref="M14">_xlfn.IFS(L14="+",ROUNDUP(K14*(1+$M$5),0),L14="=",K14)</f>
-        <v>41</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -8216,10 +8281,10 @@
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="150" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C16" s="79">
         <f>R33</f>
@@ -8263,7 +8328,7 @@
     <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="150"/>
       <c r="B17" s="91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" s="79">
         <f>T33</f>
@@ -8297,7 +8362,7 @@
         <v>71</v>
       </c>
       <c r="O17" s="149" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P17" s="149"/>
       <c r="Q17" s="149"/>
@@ -8307,7 +8372,7 @@
       </c>
       <c r="S17" s="162"/>
       <c r="T17" s="149" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="U17" s="149"/>
       <c r="V17" s="149"/>
@@ -8320,7 +8385,7 @@
     <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="150"/>
       <c r="B18" s="90" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18" s="79">
         <f>V33</f>
@@ -8379,34 +8444,34 @@
       </c>
       <c r="C19" s="79">
         <f>X33</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D19" s="75" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="79" cm="1">
         <f t="array" ref="E19">_xlfn.IFS(D19="+",ROUNDUP($C$19 * (1 +Q5) ^ 1,0),D19="=",C19)</f>
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="F19" s="75" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="79" cm="1">
         <f t="array" ref="G19">_xlfn.IFS(F19="+",ROUNDUP($C$19 * (1 +S5) ^ 2,0),F19="=",E19)</f>
-        <v>29</v>
+        <v>144</v>
       </c>
       <c r="H19" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I19" s="79" cm="1">
         <f t="array" ref="I19">_xlfn.IFS(H19="+",ROUNDDOWN(G19*(1+$Q$5),0),H19="=",G19,H19="++",ROUNDDOWN(G19*(1+$Q$5)*1.5,0),H19="-",ROUNDDOWN(G19*(1+$Q$5)*0.75,0))</f>
-        <v>65</v>
+        <v>324</v>
       </c>
       <c r="K19" s="73" t="s">
         <v>40</v>
       </c>
       <c r="M19" s="73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O19" s="164"/>
       <c r="P19" s="164"/>
@@ -8423,21 +8488,21 @@
       <c r="B20" s="16"/>
       <c r="K20" s="74" cm="1">
         <f t="array" ref="K20">_xlfn.IFS(K17="Upgrade 0",C5,K17="Upgrade 1",E5,K17="Upgrade 2",G5)</f>
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="M20" s="74" cm="1">
         <f t="array" ref="M20">_xlfn.IFS(M17="LVL 0",C14,M17="LVL 1",E14,M17="LVL 2",G14,M17="LVL 3",I14,M17="LVL 4",K14,M17="LVL 5",M14)</f>
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="O20" s="149" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P20" s="149"/>
       <c r="Q20" s="149"/>
       <c r="R20" s="162"/>
       <c r="S20" s="162"/>
       <c r="T20" s="149" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U20" s="149"/>
       <c r="V20" s="149"/>
@@ -8446,10 +8511,10 @@
     </row>
     <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="150" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" s="90" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C21" s="79">
         <f>R31</f>
@@ -8480,7 +8545,7 @@
         <v>15</v>
       </c>
       <c r="M21" s="73" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O21" s="164" t="str">
         <f>_xlfn.CONCAT(P27," ",R27," lvl ",_xlfn.CONCAT(RIGHT(M17,1)))</f>
@@ -8502,7 +8567,7 @@
     <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="150"/>
       <c r="B22" s="91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22" s="79">
         <f>T31</f>
@@ -8551,7 +8616,7 @@
     <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="150"/>
       <c r="B23" s="90" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C23" s="79">
         <f>V31</f>
@@ -8579,11 +8644,11 @@
         <v>10</v>
       </c>
       <c r="K23" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="149" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P23" s="149"/>
       <c r="Q23" s="149"/>
@@ -8597,28 +8662,28 @@
       </c>
       <c r="C24" s="79">
         <f>X31</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D24" s="75" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="79" cm="1">
         <f t="array" ref="E24">_xlfn.IFS(D24="+",ROUNDUP($C$24 * (1 +S5) ^ 1,0),D24="=",C24)</f>
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F24" s="75" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="79" cm="1">
         <f t="array" ref="G24">_xlfn.IFS(F24="+",ROUNDUP($C$19 * (1 +S5) ^ 2,0),F24="=",E24)</f>
-        <v>29</v>
+        <v>144</v>
       </c>
       <c r="H24" s="75" t="s">
         <v>13</v>
       </c>
       <c r="I24" s="79" cm="1">
         <f t="array" ref="I24">_xlfn.IFS(H24="+",ROUNDDOWN(G24*(1+$S$5),0),H24="=",G24,H24="++",ROUNDDOWN(G24*(1+$Q$5)*1.5,0),H24="-",ROUNDDOWN(G24*(1+$Q$5)*0.75,0))</f>
-        <v>34</v>
+        <v>172</v>
       </c>
       <c r="K24" s="74" cm="1">
         <f t="array" ref="K24">_xlfn.IFS(K17="Upgrade 0",C6,K17="Upgrade 1",E6,K17="Upgrade 2",G6,K17="Upgrade 3",#REF!,K17="Upgrade 4",K6,K17="Upgrade 5",M6)</f>
@@ -8681,12 +8746,12 @@
       <c r="F27" s="149"/>
       <c r="G27" s="135" t="str">
         <f>_xlfn.CONCAT(K20*K22," s")</f>
-        <v>21 s</v>
+        <v>108 s</v>
       </c>
       <c r="H27" s="135"/>
       <c r="I27" s="135"/>
       <c r="N27" s="156" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O27" s="156"/>
       <c r="P27" s="129" t="str">
@@ -8731,10 +8796,10 @@
       </c>
       <c r="F28" s="160"/>
       <c r="G28" s="73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H28" s="149" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I28" s="149"/>
       <c r="N28" s="165" t="s">
@@ -8777,11 +8842,11 @@
       </c>
       <c r="H29" s="135">
         <f>ROUNDUP(K24/M20,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29" s="135"/>
       <c r="N29" s="156" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O29" s="156"/>
       <c r="P29" s="129" t="str">
@@ -8812,7 +8877,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="N30" s="165" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O30" s="165"/>
       <c r="P30" s="165" t="s">
@@ -8820,7 +8885,7 @@
       </c>
       <c r="Q30" s="165"/>
       <c r="R30" s="165" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S30" s="165"/>
       <c r="T30" s="165" t="s">
@@ -8828,7 +8893,7 @@
       </c>
       <c r="U30" s="165"/>
       <c r="V30" s="165" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="W30" s="165"/>
       <c r="X30" s="165" t="s">
@@ -8842,7 +8907,7 @@
       </c>
       <c r="C31" s="149"/>
       <c r="N31" s="156" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O31" s="156"/>
       <c r="P31" s="129" t="str">
@@ -8867,7 +8932,7 @@
       <c r="W31" s="129"/>
       <c r="X31" s="129">
         <f>VLOOKUP($N$27,ENEMY,8)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Y31" s="129"/>
     </row>
@@ -8878,7 +8943,7 @@
       </c>
       <c r="C32" s="129"/>
       <c r="N32" s="165" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O32" s="165"/>
       <c r="P32" s="165" t="s">
@@ -8886,15 +8951,15 @@
       </c>
       <c r="Q32" s="165"/>
       <c r="R32" s="165" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S32" s="165"/>
       <c r="T32" s="165" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U32" s="165"/>
       <c r="V32" s="165" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="W32" s="165"/>
       <c r="X32" s="165" t="s">
@@ -8904,7 +8969,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="N33" s="156" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O33" s="156"/>
       <c r="P33" s="129" t="str">
@@ -8929,7 +8994,7 @@
       <c r="W33" s="129"/>
       <c r="X33" s="129">
         <f>VLOOKUP($N$29,TOWER,9)</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="Y33" s="129"/>
     </row>
@@ -10090,16 +10155,16 @@
         <v>20</v>
       </c>
       <c r="D2" s="87" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E2" s="73" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G2" s="93" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I2" s="77" t="s">
         <v>56</v>
@@ -10120,7 +10185,7 @@
         <v>69</v>
       </c>
       <c r="R2" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -10132,7 +10197,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="23">
         <v>50</v>
@@ -10147,7 +10212,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="90" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J3" s="20">
         <f>D3</f>
@@ -10187,7 +10252,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="21">
         <f>D3</f>
@@ -10206,7 +10271,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J4" s="21">
         <f>E3</f>
@@ -10246,7 +10311,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="20">
         <f>D3</f>
@@ -10265,7 +10330,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="90" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J5" s="84">
         <f>P9</f>
@@ -10330,13 +10395,13 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C7" s="149" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="149"/>
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="166" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D8" s="166"/>
       <c r="I8" s="88" t="s">
@@ -10347,7 +10412,7 @@
       </c>
       <c r="K8" s="88"/>
       <c r="L8" s="88" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M8" s="88"/>
       <c r="N8" s="88" t="s">
@@ -10355,7 +10420,7 @@
       </c>
       <c r="O8" s="88"/>
       <c r="P8" s="88" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q8" s="85"/>
     </row>
@@ -10363,7 +10428,7 @@
       <c r="C9" s="166"/>
       <c r="D9" s="166"/>
       <c r="I9" s="83" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J9" s="75" t="str">
         <f>VLOOKUP($I$9,TRAIN,3)</f>
@@ -10768,13 +10833,13 @@
         <v>20</v>
       </c>
       <c r="D2" s="87" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="73" t="s">
-        <v>147</v>
-      </c>
       <c r="F2" s="73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H2" s="77" t="s">
         <v>56</v>
@@ -10795,7 +10860,7 @@
         <v>69</v>
       </c>
       <c r="Q2" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -10807,7 +10872,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="23">
         <v>100</v>
@@ -10819,7 +10884,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="90" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I3" s="20">
         <f>D3</f>
@@ -10859,7 +10924,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="21">
         <f>D3</f>
@@ -10874,7 +10939,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I4" s="21">
         <f>E3</f>
@@ -10914,7 +10979,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="20">
         <f>D3</f>
@@ -10929,7 +10994,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="90" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I5" s="20">
         <f>F3</f>
@@ -10994,16 +11059,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C7" s="149" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="149"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" s="166" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" s="166" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H8" s="88" t="s">
         <v>33</v>
@@ -11013,15 +11078,15 @@
       </c>
       <c r="J8" s="88"/>
       <c r="K8" s="88" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L8" s="88"/>
       <c r="M8" s="88" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N8" s="88"/>
       <c r="O8" s="88" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P8" s="88"/>
     </row>
@@ -11029,7 +11094,7 @@
       <c r="C9" s="166"/>
       <c r="D9" s="166"/>
       <c r="H9" s="83" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I9" s="75" t="str">
         <f>VLOOKUP($H$9,FACTORY,3)</f>
@@ -11207,7 +11272,7 @@
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="K12" sqref="K12:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11310,7 +11375,7 @@
         <v>39</v>
       </c>
       <c r="I2" s="87" t="s">
-        <v>80</v>
+        <v>213</v>
       </c>
       <c r="K2" s="151" t="s">
         <v>56</v>
@@ -11342,7 +11407,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>50</v>
@@ -11360,7 +11425,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="23">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="K3" s="150" t="s">
         <v>45</v>
@@ -11370,21 +11435,21 @@
       </c>
       <c r="M3" s="51">
         <f>$Q$12</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N3" s="28" t="s">
         <v>13</v>
       </c>
       <c r="O3" s="28" cm="1">
         <f t="array" ref="O3">_xlfn.IFS(N3="+",ROUNDDOWN(M3*(1+$T$3),2),N3="=",M3)</f>
-        <v>3.9</v>
+        <v>5.2</v>
       </c>
       <c r="P3" s="28" t="s">
         <v>13</v>
       </c>
       <c r="Q3" s="28" cm="1">
         <f t="array" ref="Q3">_xlfn.IFS(P3="+",ROUNDDOWN(O3*(1+$T$3),2),P3="=",O3)</f>
-        <v>5.07</v>
+        <v>6.76</v>
       </c>
       <c r="R3" s="28" t="s">
         <v>13</v>
@@ -11403,7 +11468,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>52</v>
@@ -11421,8 +11486,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="21">
-        <f>I3</f>
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K4" s="150"/>
       <c r="L4" s="91" t="s">
@@ -11430,21 +11494,21 @@
       </c>
       <c r="M4" s="29">
         <f>$S$12</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="N4" s="29" t="s">
         <v>13</v>
       </c>
       <c r="O4" s="29" cm="1">
         <f t="array" ref="O4">_xlfn.IFS(N4="+",ROUNDDOWN(M4*(1-$T$4),2),N4="=",M4)</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="P4" s="29" t="s">
         <v>13</v>
       </c>
       <c r="Q4" s="29" cm="1">
         <f t="array" ref="Q4">_xlfn.IFS(P4="+",ROUNDDOWN(O4*(1-$T$4),2),P4="=",O4)</f>
-        <v>0.48</v>
+        <v>0.64</v>
       </c>
       <c r="R4" s="29" t="s">
         <v>13</v>
@@ -11463,7 +11527,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>51</v>
@@ -11481,8 +11545,7 @@
         <v>20</v>
       </c>
       <c r="I5" s="20">
-        <f>I3</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="K5" s="150"/>
       <c r="L5" s="90" t="s">
@@ -11490,21 +11553,21 @@
       </c>
       <c r="M5" s="28">
         <f>$U$12</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="N5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="O5" s="28" cm="1">
         <f t="array" ref="O5">_xlfn.IFS(N5="+",ROUNDDOWN(M5*(1+$T$5),2),N5="=",M5)</f>
-        <v>3.85</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="P5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="Q5" s="28" cm="1">
         <f t="array" ref="Q5">_xlfn.IFS(P5="+",ROUNDDOWN(O5*(1+$T$5),2),P5="=",O5)</f>
-        <v>4.2300000000000004</v>
+        <v>4.84</v>
       </c>
       <c r="R5" s="28" t="s">
         <v>13</v>
@@ -11546,7 +11609,7 @@
       </c>
       <c r="I6" s="21">
         <f>I3</f>
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="K6" s="150"/>
       <c r="L6" s="91" t="s">
@@ -11554,21 +11617,21 @@
       </c>
       <c r="M6" s="29">
         <f>$W$12</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N6" s="29" t="s">
         <v>13</v>
       </c>
       <c r="O6" s="29" cm="1">
         <f t="array" ref="O6">_xlfn.IFS(N6="+",ROUNDDOWN(M6*(1+$T$6),0),N6="=",M6)</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="P6" s="29" t="s">
         <v>13</v>
       </c>
       <c r="Q6" s="29" cm="1">
         <f t="array" ref="Q6">_xlfn.IFS(P6="+",ROUNDDOWN(O6*(1+$T$6),0),P6="=",O6)</f>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="R6" s="29" t="s">
         <v>13</v>
@@ -11609,28 +11672,29 @@
         <v>15</v>
       </c>
       <c r="I7" s="20">
-        <f>I3</f>
-        <v>20</v>
+        <f>I4</f>
+        <v>80</v>
       </c>
       <c r="K7" s="150"/>
       <c r="L7" s="90" t="s">
         <v>78</v>
       </c>
       <c r="M7" s="28">
-        <v>10</v>
+        <f>ROUNDUP(VLOOKUP(K12,TOWER,9,FALSE)/2,0)</f>
+        <v>40</v>
       </c>
       <c r="N7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="28" cm="1">
-        <f t="array" ref="O7">_xlfn.IFS(N7="+",ROUNDUP(M7*(1+$T$7),0),N7="=",M7)</f>
-        <v>30</v>
-      </c>
-      <c r="P7" s="28" t="s">
+      <c r="O7" s="28">
+        <f>MROUND(M7+ROUNDUP(M7/2,0),5)</f>
+        <v>60</v>
+      </c>
+      <c r="P7" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="28" cm="1">
-        <f t="array" ref="Q7">_xlfn.IFS(P7="+",ROUNDUP(O7*(1+$T$7),0),P7="=",O7)</f>
+      <c r="Q7" s="94">
+        <f>MROUND(O7+ROUNDUP(O7/2,0),5)</f>
         <v>90</v>
       </c>
       <c r="R7" s="28" t="s">
@@ -11672,8 +11736,8 @@
         <v>20</v>
       </c>
       <c r="I8" s="21">
-        <f>I3</f>
-        <v>20</v>
+        <f>I5</f>
+        <v>100</v>
       </c>
       <c r="K8" s="169" t="s">
         <v>60</v>
@@ -11681,12 +11745,12 @@
       <c r="L8" s="169"/>
       <c r="M8" s="28">
         <f>ROUNDDOWN(M3*M9,2)</f>
-        <v>3.99</v>
+        <v>4</v>
       </c>
       <c r="N8" s="28"/>
       <c r="O8" s="28">
         <f>ROUNDDOWN(O3*O9,2)</f>
-        <v>6.51</v>
+        <v>6.5</v>
       </c>
       <c r="P8" s="28"/>
       <c r="Q8" s="28">
@@ -11727,7 +11791,7 @@
       </c>
       <c r="I9" s="20">
         <f>I3</f>
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="K9" s="170" t="s">
         <v>46</v>
@@ -11735,17 +11799,17 @@
       <c r="L9" s="170"/>
       <c r="M9" s="29">
         <f>ROUNDDOWN(1/M4,2)</f>
-        <v>1.33</v>
+        <v>1</v>
       </c>
       <c r="N9" s="29"/>
       <c r="O9" s="29">
         <f>ROUND(1/O4,2)</f>
-        <v>1.67</v>
+        <v>1.25</v>
       </c>
       <c r="P9" s="29"/>
       <c r="Q9" s="29">
         <f>ROUND(1/Q4,2)</f>
-        <v>2.08</v>
+        <v>1.56</v>
       </c>
       <c r="R9" s="29"/>
     </row>
@@ -11780,8 +11844,8 @@
         <v>15</v>
       </c>
       <c r="I10" s="21">
-        <f>I3</f>
-        <v>20</v>
+        <f>I4</f>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -11815,8 +11879,8 @@
         <v>20</v>
       </c>
       <c r="I11" s="20">
-        <f>I3</f>
-        <v>20</v>
+        <f>I5</f>
+        <v>100</v>
       </c>
       <c r="K11" s="165" t="s">
         <v>41</v>
@@ -11847,63 +11911,63 @@
       </c>
       <c r="X11" s="165"/>
       <c r="Y11" s="165" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z11" s="165"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K12" s="156" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="L12" s="156"/>
       <c r="M12" s="129" t="str">
         <f>VLOOKUP($K$12,TOWER,3)</f>
-        <v>Traps</v>
+        <v>Pizza</v>
       </c>
       <c r="N12" s="129"/>
       <c r="O12" s="129" t="str">
         <f>VLOOKUP($K$12,TOWER,4)</f>
-        <v>Canon</v>
+        <v>Mortar</v>
       </c>
       <c r="P12" s="129"/>
       <c r="Q12" s="129">
         <f>VLOOKUP($K$12,TOWER,5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R12" s="129"/>
       <c r="S12" s="129">
         <f>VLOOKUP($K$12,TOWER,6)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="T12" s="129"/>
       <c r="U12" s="129">
         <f>VLOOKUP($K$12,TOWER,7)</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="V12" s="129"/>
       <c r="W12" s="129">
         <f>VLOOKUP($K$12,TOWER,8)</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="X12" s="129"/>
       <c r="Y12" s="129">
         <f>VLOOKUP($K$12,TOWER,9)</f>
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z12" s="129"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C13" s="168" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="168"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C14" s="166" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" s="166" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -11982,7 +12046,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L10" xr:uid="{E6E8CE4E-28A1-4DB8-B138-1D7059EC2372}">
       <formula1>STAT_TOWER</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R10 P3:P10 N3:N10 T8:T10 V3:V10" xr:uid="{C77BBF24-DFCE-4151-AAA2-8695D03BF95B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R10 V3:V10 N3:N10 T8:T10 P3:P10" xr:uid="{C77BBF24-DFCE-4151-AAA2-8695D03BF95B}">
       <formula1>SIGN</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12" xr:uid="{A91C467D-D990-41FA-81A0-203403B29185}">
@@ -12006,7 +12070,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>N3:N7 P3:P7 R3:R7</xm:sqref>
+          <xm:sqref>N3:N7 R3:R7 P3:P7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="1" operator="containsText" id="{5A627A3F-8B8B-4B82-9DE7-0E87BD6E5ED1}">
@@ -12020,7 +12084,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>N3:N7 P3:P7 R3:R7</xm:sqref>
+          <xm:sqref>N3:N7 R3:R7 P3:P7</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -12033,7 +12097,7 @@
   <dimension ref="A1:X18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F22"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12147,7 +12211,7 @@
         <v>62</v>
       </c>
       <c r="H2" s="73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I2" s="46"/>
       <c r="J2" s="77" t="s">
@@ -12205,7 +12269,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="23">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I3" s="47"/>
       <c r="J3" s="76" t="s">
@@ -12279,7 +12343,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="23">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I4" s="47"/>
       <c r="J4" s="77" t="s">
@@ -12353,7 +12417,7 @@
         <v>7.5</v>
       </c>
       <c r="H5" s="23">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J5" s="76" t="s">
         <v>72</v>
@@ -12430,49 +12494,49 @@
       </c>
       <c r="H6" s="21">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J6" s="77" t="s">
         <v>75</v>
       </c>
       <c r="K6" s="21">
         <f>U9</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="M6" s="21" cm="1">
         <f t="array" ref="M6">_xlfn.IFS(L6="+",ROUNDDOWN($K$6 * (1 + W6) ^ 1,2),L6="=",K6)</f>
-        <v>4.5</v>
+        <v>12</v>
       </c>
       <c r="N6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="O6" s="21" cm="1">
         <f t="array" ref="O6">_xlfn.IFS(L6="+",ROUNDDOWN($K$6 * (1 + W6) ^ 2,2),L6="=",K6)</f>
-        <v>6.75</v>
+        <v>18</v>
       </c>
       <c r="P6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="Q6" s="21" cm="1">
         <f t="array" ref="Q6">_xlfn.IFS(L6="+",ROUNDDOWN($K$6 * (1 + W6) ^ 3,2),L6="=",K6)</f>
-        <v>10.119999999999999</v>
+        <v>27</v>
       </c>
       <c r="R6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="S6" s="21" cm="1">
         <f t="array" ref="S6">_xlfn.IFS(L6="+",ROUNDDOWN($K$6 * (1 + W6) ^ 4,2),L6="=",K6)</f>
-        <v>15.18</v>
+        <v>40.5</v>
       </c>
       <c r="T6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="U6" s="21" cm="1">
         <f t="array" ref="U6">_xlfn.IFS(L6="+",ROUNDDOWN($K$6 * (1 + W6) ^ 5,2),L6="=",K6)</f>
-        <v>22.78</v>
+        <v>60.75</v>
       </c>
       <c r="V6" s="14"/>
       <c r="W6" s="11">
@@ -12507,7 +12571,7 @@
       </c>
       <c r="H7" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -12538,7 +12602,7 @@
       </c>
       <c r="H8" s="21">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J8" s="88" t="s">
         <v>33</v>
@@ -12595,10 +12659,10 @@
       </c>
       <c r="H9" s="20">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J9" s="83" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K9" s="75" t="str">
         <f>VLOOKUP($J$9,ENEMY,3)</f>
@@ -12627,7 +12691,7 @@
       <c r="T9" s="75"/>
       <c r="U9" s="75">
         <f>VLOOKUP($J$9,ENEMY,8)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -12658,7 +12722,7 @@
       </c>
       <c r="H10" s="21">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -12689,7 +12753,7 @@
       </c>
       <c r="H11" s="20">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -12697,16 +12761,16 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C13" s="149" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="149"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C14" s="166" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" s="166" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -12935,7 +12999,7 @@
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="31"/>
       <c r="C2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
@@ -12961,7 +13025,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="121" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H3" s="122" t="s">
         <v>25</v>
@@ -13098,7 +13162,7 @@
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C12" s="172" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D12" s="172"/>
       <c r="E12" s="172"/>
@@ -13124,10 +13188,10 @@
         <v>72</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>14</v>
@@ -13139,16 +13203,16 @@
         <v>13</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O13" s="172" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P13" s="172"/>
     </row>
     <row r="14" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -13166,7 +13230,7 @@
         <v>72</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J14" s="54">
         <f>COUNTIF(C14:E14,"=-")</f>
@@ -13195,13 +13259,13 @@
     </row>
     <row r="15" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>12</v>
@@ -13238,7 +13302,7 @@
     </row>
     <row r="16" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="63" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
@@ -13247,7 +13311,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F16" s="30">
         <v>3</v>
@@ -13278,7 +13342,7 @@
     </row>
     <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -13316,7 +13380,7 @@
     </row>
     <row r="18" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>14</v>
@@ -13325,7 +13389,7 @@
         <v>12</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F18" s="30">
         <v>5</v>
@@ -13354,10 +13418,10 @@
     </row>
     <row r="19" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>14</v>
@@ -13392,7 +13456,7 @@
     </row>
     <row r="20" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
@@ -13430,10 +13494,10 @@
     </row>
     <row r="21" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>14</v>
@@ -13468,13 +13532,13 @@
     </row>
     <row r="22" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
@@ -13557,7 +13621,7 @@
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27" s="54">
         <f>COUNTIF(C14:C22,"=++")</f>
@@ -13596,7 +13660,7 @@
     </row>
     <row r="31" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="172" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D31" s="172"/>
       <c r="E31" s="172"/>
@@ -13962,30 +14026,30 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="176" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="176" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="176" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="176" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="176" t="s">
+      <c r="E1" s="176" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="176" t="s">
+      <c r="F1" s="176" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="176" t="s">
+      <c r="G1" s="177" t="s">
         <v>99</v>
-      </c>
-      <c r="G1" s="177" t="s">
-        <v>100</v>
       </c>
       <c r="H1" s="178"/>
       <c r="I1" s="179"/>
       <c r="J1" s="175" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K1" s="175"/>
       <c r="L1" s="175"/>
@@ -14001,19 +14065,19 @@
         <v>72</v>
       </c>
       <c r="H2" s="92" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="I2" s="92" t="s">
+      <c r="J2" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="92" t="s">
+      <c r="K2" s="92" t="s">
         <v>104</v>
       </c>
-      <c r="K2" s="92" t="s">
+      <c r="L2" s="92" t="s">
         <v>105</v>
-      </c>
-      <c r="L2" s="92" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -14031,10 +14095,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="59" t="s">
         <v>107</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>108</v>
       </c>
       <c r="G3" s="57" t="s">
         <v>12</v>
@@ -14061,19 +14125,19 @@
         <v>36</v>
       </c>
       <c r="D4" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="F4" s="60" t="s">
         <v>110</v>
-      </c>
-      <c r="F4" s="60" t="s">
-        <v>111</v>
       </c>
       <c r="G4" s="58" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I4" s="58" t="s">
         <v>12</v>
@@ -14094,13 +14158,13 @@
         <v>36</v>
       </c>
       <c r="D5" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="F5" s="59" t="s">
         <v>114</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>115</v>
       </c>
       <c r="G5" s="57" t="s">
         <v>14</v>
@@ -14109,7 +14173,7 @@
         <v>12</v>
       </c>
       <c r="I5" s="68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
@@ -14130,10 +14194,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G6" s="58" t="s">
         <v>13</v>
@@ -14160,13 +14224,13 @@
         <v>8</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="59" t="s">
         <v>117</v>
-      </c>
-      <c r="F7" s="59" t="s">
-        <v>118</v>
       </c>
       <c r="G7" s="57" t="s">
         <v>14</v>
@@ -14175,7 +14239,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
@@ -14193,16 +14257,16 @@
         <v>8</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="F8" s="60" t="s">
-        <v>120</v>
-      </c>
       <c r="G8" s="67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H8" s="58" t="s">
         <v>14</v>
@@ -14223,16 +14287,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="21">
         <v>1</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G9" s="57" t="s">
         <v>13</v>
@@ -14256,19 +14320,19 @@
         <v>8</v>
       </c>
       <c r="C10" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" s="20" t="s">
+      <c r="F10" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="F10" s="60" t="s">
-        <v>123</v>
-      </c>
       <c r="G10" s="58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H10" s="58" t="s">
         <v>14</v>
@@ -14289,22 +14353,22 @@
         <v>9</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="59" t="s">
         <v>124</v>
-      </c>
-      <c r="F11" s="59" t="s">
-        <v>125</v>
       </c>
       <c r="G11" s="57" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I11" s="57" t="s">
         <v>14</v>
@@ -14318,15 +14382,15 @@
         <v>72</v>
       </c>
       <c r="H13" s="55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I13" s="55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F14" s="156" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G14" s="129" t="str">
         <f>VLOOKUP($F$14,TOWER_UPGRADE,7)</f>
@@ -14459,16 +14523,16 @@
         <v>17</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>58</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -14477,7 +14541,7 @@
       </c>
       <c r="C3" s="35"/>
       <c r="D3" s="66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="35"/>
       <c r="F3" s="36" t="s">
@@ -14490,7 +14554,7 @@
         <v>44</v>
       </c>
       <c r="L3" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -14509,10 +14573,10 @@
         <v>44</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14534,7 +14598,7 @@
         <v>40</v>
       </c>
       <c r="L5" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14588,7 +14652,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H10" s="37" t="s">
         <v>24</v>
@@ -14682,7 +14746,7 @@
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -14692,18 +14756,18 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -14718,12 +14782,12 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify System design ADD Waves Test
</commit_message>
<xml_diff>
--- a/Documents/GameDesign/System_Design.xlsx
+++ b/Documents/GameDesign/System_Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GameSup_GD1\Workshop\Tower_Defense\STD_Workshop\Documents\GameDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE107A02-1301-4EF3-99DE-7B97B78D6295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFBDED7-46BC-4A9C-B4C9-E3580CD99E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{EE4EEEAB-A39E-4793-9971-E358DB8AAF6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{EE4EEEAB-A39E-4793-9971-E358DB8AAF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Wave" sheetId="10" r:id="rId1"/>
@@ -5215,8 +5215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECF5610-AFF3-4403-B872-F795309595A3}">
   <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5849,9 +5849,15 @@
       <c r="P11" s="116"/>
       <c r="Q11" s="94"/>
       <c r="R11" s="117"/>
-      <c r="S11" s="116"/>
-      <c r="T11" s="94"/>
-      <c r="U11" s="117"/>
+      <c r="S11" s="116">
+        <v>1</v>
+      </c>
+      <c r="T11" s="94">
+        <v>1</v>
+      </c>
+      <c r="U11" s="117">
+        <v>1</v>
+      </c>
       <c r="V11" s="116"/>
       <c r="W11" s="94"/>
       <c r="X11" s="117"/>
@@ -5970,7 +5976,7 @@
       <c r="R14" s="133"/>
       <c r="S14" s="131">
         <f>S3*T3*VLOOKUP($B$3,ENEMY,7)+S4*T4*VLOOKUP($B$4,ENEMY,7)+S5*T5*VLOOKUP($B$5,ENEMY,7)+S6*T6*VLOOKUP($B$6,ENEMY,7)+S7*T7*VLOOKUP($B$7,ENEMY,7)+S8*T8*VLOOKUP($B$8,ENEMY,7)+S9*T9*VLOOKUP($B$9,ENEMY,7)+S10*T10*VLOOKUP($B$10,ENEMY,7)+S11*T11*VLOOKUP($B$11,ENEMY,7)</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="T14" s="132"/>
       <c r="U14" s="133"/>
@@ -6192,37 +6198,37 @@
       <c r="U18" s="130"/>
       <c r="V18" s="128">
         <f t="shared" ref="V18" si="9">S22</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="W18" s="129"/>
       <c r="X18" s="130"/>
       <c r="Y18" s="128">
         <f t="shared" ref="Y18" si="10">V22</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="Z18" s="129"/>
       <c r="AA18" s="130"/>
       <c r="AB18" s="128">
         <f t="shared" ref="AB18" si="11">Y22</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="AC18" s="129"/>
       <c r="AD18" s="130"/>
       <c r="AE18" s="128">
         <f t="shared" ref="AE18" si="12">AB22</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="AF18" s="129"/>
       <c r="AG18" s="130"/>
       <c r="AH18" s="128">
         <f t="shared" ref="AH18" si="13">AE22</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="AI18" s="129"/>
       <c r="AJ18" s="130"/>
       <c r="AK18" s="128">
         <f t="shared" ref="AK18" si="14">AH22</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="AL18" s="129"/>
       <c r="AM18" s="130"/>
@@ -6417,7 +6423,7 @@
       <c r="R21" s="136"/>
       <c r="S21" s="134">
         <f>S3*T3*VLOOKUP($B$3,ENEMY,8)+S4*T4*VLOOKUP($B$4,ENEMY,8)+S5*T5*VLOOKUP($B$5,ENEMY,8)+S6*T6*VLOOKUP($B$6,ENEMY,8)+S7*T7*VLOOKUP($B$7,ENEMY,8)+S8*T8*VLOOKUP($B$8,ENEMY,8)+S9*T9*VLOOKUP($B$9,ENEMY,8)+S10*T10*VLOOKUP($B$10,ENEMY,8)+S11*T11*VLOOKUP($B$11,ENEMY,8)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T21" s="135"/>
       <c r="U21" s="136"/>
@@ -6494,43 +6500,43 @@
       <c r="R22" s="130"/>
       <c r="S22" s="128">
         <f t="shared" ref="S22" si="18">S18-(S19+S20)+S21</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="T22" s="129"/>
       <c r="U22" s="130"/>
       <c r="V22" s="128">
         <f t="shared" ref="V22" si="19">V18-(V19+V20)+V21</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="W22" s="129"/>
       <c r="X22" s="130"/>
       <c r="Y22" s="128">
         <f t="shared" ref="Y22" si="20">Y18-(Y19+Y20)+Y21</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="Z22" s="129"/>
       <c r="AA22" s="130"/>
       <c r="AB22" s="128">
         <f t="shared" ref="AB22" si="21">AB18-(AB19+AB20)+AB21</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="AC22" s="129"/>
       <c r="AD22" s="130"/>
       <c r="AE22" s="128">
         <f t="shared" ref="AE22" si="22">AE18-(AE19+AE20)+AE21</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="AF22" s="129"/>
       <c r="AG22" s="130"/>
       <c r="AH22" s="128">
         <f t="shared" ref="AH22" si="23">AH18-(AH19+AH20)+AH21</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="AI22" s="129"/>
       <c r="AJ22" s="130"/>
       <c r="AK22" s="128">
         <f t="shared" ref="AK22" si="24">AK18-(AK19+AK20)+AK21</f>
-        <v>-89</v>
+        <v>-69</v>
       </c>
       <c r="AL22" s="129"/>
       <c r="AM22" s="130"/>
@@ -10755,7 +10761,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11272,7 +11278,7 @@
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12:L12"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12097,7 +12103,7 @@
   <dimension ref="A1:X18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12986,8 +12992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483C23BD-B808-464E-B86B-8B4FE0CBBEE3}">
   <dimension ref="B2:P38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>